<commit_message>
added new plots and updated the code eqns
</commit_message>
<xml_diff>
--- a/GK_Data_M1_filled.xlsx
+++ b/GK_Data_M1_filled.xlsx
@@ -529,16 +529,16 @@
         <v>0.09</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0136138275</v>
+        <v>0.00136138275</v>
       </c>
       <c r="F2" t="n">
         <v>0.45</v>
       </c>
       <c r="G2" t="n">
-        <v>0.07684181716202555</v>
+        <v>0.007684181716202553</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1707595936933901</v>
+        <v>0.01707595936933901</v>
       </c>
       <c r="I2" t="n">
         <v>14.1</v>
@@ -556,7 +556,7 @@
         <v>0.02500404967200313</v>
       </c>
       <c r="N2" t="n">
-        <v>3.302854366862582e-05</v>
+        <v>3.302854366862581e-06</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -581,16 +581,16 @@
         <v>0.38</v>
       </c>
       <c r="E3" t="n">
-        <v>0.19388484</v>
+        <v>0.019388484</v>
       </c>
       <c r="F3" t="n">
         <v>1.9</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2659768058574089</v>
+        <v>0.02659768058574088</v>
       </c>
       <c r="H3" t="n">
-        <v>0.139987792556531</v>
+        <v>0.0139987792556531</v>
       </c>
       <c r="I3" t="n">
         <v>14.1</v>
@@ -608,7 +608,7 @@
         <v>0.02507209604321107</v>
       </c>
       <c r="N3" t="n">
-        <v>9.353065580141351e-05</v>
+        <v>9.353065580141349e-06</v>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
@@ -629,16 +629,16 @@
         <v>0.22</v>
       </c>
       <c r="E4" t="n">
-        <v>0.09589520250000001</v>
+        <v>0.009589520249999999</v>
       </c>
       <c r="F4" t="n">
         <v>1.1</v>
       </c>
       <c r="G4" t="n">
-        <v>0.3635248208507968</v>
+        <v>0.03635248208507967</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3304771098643607</v>
+        <v>0.03304771098643606</v>
       </c>
       <c r="I4" t="n">
         <v>14.1</v>
@@ -656,7 +656,7 @@
         <v>0.02502418829852429</v>
       </c>
       <c r="N4" t="n">
-        <v>7.06384215410706e-05</v>
+        <v>7.063842154107058e-06</v>
       </c>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
@@ -677,16 +677,16 @@
         <v>0.13</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03336135750000001</v>
+        <v>0.00333613575</v>
       </c>
       <c r="F5" t="n">
         <v>0.65</v>
       </c>
       <c r="G5" t="n">
-        <v>0.1669937543796806</v>
+        <v>0.01669937543796805</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2569134682764316</v>
+        <v>0.02569134682764316</v>
       </c>
       <c r="I5" t="n">
         <v>14.1</v>
@@ -704,7 +704,7 @@
         <v>0.02500844857243248</v>
       </c>
       <c r="N5" t="n">
-        <v>5.026536750154372e-05</v>
+        <v>5.026536750154372e-06</v>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
@@ -725,16 +725,16 @@
         <v>0.1</v>
       </c>
       <c r="E6" t="n">
-        <v>0.019448325</v>
+        <v>0.0019448325</v>
       </c>
       <c r="F6" t="n">
         <v>0.5</v>
       </c>
       <c r="G6" t="n">
-        <v>0.1057007768542042</v>
+        <v>0.01057007768542042</v>
       </c>
       <c r="H6" t="n">
-        <v>0.2114015537084084</v>
+        <v>0.02114015537084084</v>
       </c>
       <c r="I6" t="n">
         <v>14.1</v>
@@ -752,7 +752,7 @@
         <v>0.02500499950009998</v>
       </c>
       <c r="N6" t="n">
-        <v>3.988212794490945e-05</v>
+        <v>3.988212794490943e-06</v>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
@@ -773,16 +773,16 @@
         <v>0.23</v>
       </c>
       <c r="E7" t="n">
-        <v>0.09035991</v>
+        <v>0.009035990999999998</v>
       </c>
       <c r="F7" t="n">
         <v>1.15</v>
       </c>
       <c r="G7" t="n">
-        <v>0.2375079379606459</v>
+        <v>0.02375079379606458</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2065286417049094</v>
+        <v>0.02065286417049094</v>
       </c>
       <c r="I7" t="n">
         <v>14.1</v>
@@ -800,7 +800,7 @@
         <v>0.02502643602273404</v>
       </c>
       <c r="N7" t="n">
-        <v>6.931342925812443e-05</v>
+        <v>6.931342925812441e-06</v>
       </c>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="n">
@@ -821,16 +821,16 @@
         <v>0.34</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1617203025</v>
+        <v>0.01617203025</v>
       </c>
       <c r="F8" t="n">
         <v>1.7</v>
       </c>
       <c r="G8" t="n">
-        <v>0.3149967748475978</v>
+        <v>0.03149967748475978</v>
       </c>
       <c r="H8" t="n">
-        <v>0.1852922204985869</v>
+        <v>0.0185292220498587</v>
       </c>
       <c r="I8" t="n">
         <v>14.1</v>
@@ -848,7 +848,7 @@
         <v>0.02505773333723544</v>
       </c>
       <c r="N8" t="n">
-        <v>8.58320887119166e-05</v>
+        <v>8.58320887119166e-06</v>
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
@@ -869,16 +869,16 @@
         <v>0.35</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1677044025</v>
+        <v>0.01677044025</v>
       </c>
       <c r="F9" t="n">
         <v>1.75</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3126029585287417</v>
+        <v>0.03126029585287416</v>
       </c>
       <c r="H9" t="n">
-        <v>0.1786302620164238</v>
+        <v>0.01786302620164238</v>
       </c>
       <c r="I9" t="n">
         <v>14.1</v>
@@ -896,7 +896,7 @@
         <v>0.02506117515201552</v>
       </c>
       <c r="N9" t="n">
-        <v>8.724091891729097e-05</v>
+        <v>8.724091891729096e-06</v>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
@@ -917,16 +917,16 @@
         <v>0.18</v>
       </c>
       <c r="E10" t="n">
-        <v>0.06791953500000002</v>
+        <v>0.006791953500000001</v>
       </c>
       <c r="F10" t="n">
         <v>0.8999999999999999</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2923244517019918</v>
+        <v>0.02923244517019918</v>
       </c>
       <c r="H10" t="n">
-        <v>0.3248049463355465</v>
+        <v>0.03248049463355464</v>
       </c>
       <c r="I10" t="n">
         <v>14.1</v>
@@ -944,7 +944,7 @@
         <v>0.02501619475459847</v>
       </c>
       <c r="N10" t="n">
-        <v>6.350649824631214e-05</v>
+        <v>6.350649824631214e-06</v>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
@@ -965,16 +965,16 @@
         <v>0.41</v>
       </c>
       <c r="E11" t="n">
-        <v>0.1943336475</v>
+        <v>0.01943336475</v>
       </c>
       <c r="F11" t="n">
         <v>2.05</v>
       </c>
       <c r="G11" t="n">
-        <v>0.2442068637325234</v>
+        <v>0.02442068637325234</v>
       </c>
       <c r="H11" t="n">
-        <v>0.1191252993817187</v>
+        <v>0.01191252993817187</v>
       </c>
       <c r="I11" t="n">
         <v>14.1</v>
@@ -992,7 +992,7 @@
         <v>0.02508390918497354</v>
       </c>
       <c r="N11" t="n">
-        <v>9.364034534898302e-05</v>
+        <v>9.364034534898301e-06</v>
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
@@ -1013,16 +1013,16 @@
         <v>0.45</v>
       </c>
       <c r="E12" t="n">
-        <v>0.2039082075</v>
+        <v>0.02039082075</v>
       </c>
       <c r="F12" t="n">
         <v>2.25</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2071262102960011</v>
+        <v>0.0207126210296001</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0920560934648894</v>
+        <v>0.009205609346488935</v>
       </c>
       <c r="I12" t="n">
         <v>14.1</v>
@@ -1040,7 +1040,7 @@
         <v>0.02510104579494647</v>
       </c>
       <c r="N12" t="n">
-        <v>9.599559855410409e-05</v>
+        <v>9.599559855410405e-06</v>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
@@ -1061,16 +1061,16 @@
         <v>0.22</v>
       </c>
       <c r="E13" t="n">
-        <v>0.09050951250000001</v>
+        <v>0.00905095125</v>
       </c>
       <c r="F13" t="n">
         <v>1.1</v>
       </c>
       <c r="G13" t="n">
-        <v>0.5743749194909871</v>
+        <v>0.05743749194909869</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5221590177190791</v>
+        <v>0.05221590177190789</v>
       </c>
       <c r="I13" t="n">
         <v>14.1</v>
@@ -1088,7 +1088,7 @@
         <v>0.02502418829852429</v>
       </c>
       <c r="N13" t="n">
-        <v>6.934960335699357e-05</v>
+        <v>6.934960335699356e-06</v>
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
@@ -1109,16 +1109,16 @@
         <v>0.18</v>
       </c>
       <c r="E14" t="n">
-        <v>0.05909298750000001</v>
+        <v>0.005909298749999999</v>
       </c>
       <c r="F14" t="n">
         <v>0.8999999999999999</v>
       </c>
       <c r="G14" t="n">
-        <v>0.2648550961163741</v>
+        <v>0.02648550961163741</v>
       </c>
       <c r="H14" t="n">
-        <v>0.2942834401293046</v>
+        <v>0.02942834401293046</v>
       </c>
       <c r="I14" t="n">
         <v>14.1</v>
@@ -1136,7 +1136,7 @@
         <v>0.02501619475459847</v>
       </c>
       <c r="N14" t="n">
-        <v>6.087358782233311e-05</v>
+        <v>6.087358782233309e-06</v>
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
@@ -1157,16 +1157,16 @@
         <v>0.14</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0417390975</v>
+        <v>0.00417390975</v>
       </c>
       <c r="F15" t="n">
         <v>0.7000000000000001</v>
       </c>
       <c r="G15" t="n">
-        <v>0.2019359527931409</v>
+        <v>0.02019359527931409</v>
       </c>
       <c r="H15" t="n">
-        <v>0.2884799325616298</v>
+        <v>0.02884799325616299</v>
       </c>
       <c r="I15" t="n">
         <v>14.1</v>
@@ -1184,7 +1184,7 @@
         <v>0.02500979807995259</v>
       </c>
       <c r="N15" t="n">
-        <v>5.444869769922636e-05</v>
+        <v>5.444869769922636e-06</v>
       </c>
       <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
@@ -1205,16 +1205,16 @@
         <v>0.12</v>
       </c>
       <c r="E16" t="n">
-        <v>0.03021970500000001</v>
+        <v>0.0030219705</v>
       </c>
       <c r="F16" t="n">
         <v>0.6</v>
       </c>
       <c r="G16" t="n">
-        <v>0.1531666451975965</v>
+        <v>0.01531666451975965</v>
       </c>
       <c r="H16" t="n">
-        <v>0.2552777419959942</v>
+        <v>0.02552777419959942</v>
       </c>
       <c r="I16" t="n">
         <v>14.1</v>
@@ -1232,7 +1232,7 @@
         <v>0.02500719896349849</v>
       </c>
       <c r="N16" t="n">
-        <v>4.839150393208288e-05</v>
+        <v>4.839150393208287e-06</v>
       </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
@@ -1253,16 +1253,16 @@
         <v>0.11</v>
       </c>
       <c r="E17" t="n">
-        <v>0.02528282250000001</v>
+        <v>0.00252828225</v>
       </c>
       <c r="F17" t="n">
         <v>0.55</v>
       </c>
       <c r="G17" t="n">
-        <v>0.1323805490466912</v>
+        <v>0.01323805490466913</v>
       </c>
       <c r="H17" t="n">
-        <v>0.2406919073576204</v>
+        <v>0.02406919073576204</v>
       </c>
       <c r="I17" t="n">
         <v>14.1</v>
@@ -1280,7 +1280,7 @@
         <v>0.02500604926812711</v>
       </c>
       <c r="N17" t="n">
-        <v>4.497132727975271e-05</v>
+        <v>4.497132727975271e-06</v>
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
@@ -1301,16 +1301,16 @@
         <v>0.11</v>
       </c>
       <c r="E18" t="n">
-        <v>0.02094435</v>
+        <v>0.002094435</v>
       </c>
       <c r="F18" t="n">
         <v>0.55</v>
       </c>
       <c r="G18" t="n">
-        <v>0.1114189899195347</v>
+        <v>0.01114189899195346</v>
       </c>
       <c r="H18" t="n">
-        <v>0.2025799816718812</v>
+        <v>0.02025799816718812</v>
       </c>
       <c r="I18" t="n">
         <v>14.1</v>
@@ -1328,7 +1328,7 @@
         <v>0.02500604926812711</v>
       </c>
       <c r="N18" t="n">
-        <v>4.132234080552283e-05</v>
+        <v>4.132234080552282e-06</v>
       </c>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
@@ -1349,16 +1349,16 @@
         <v>0.1</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0184011075</v>
+        <v>0.00184011075</v>
       </c>
       <c r="F19" t="n">
         <v>0.5</v>
       </c>
       <c r="G19" t="n">
-        <v>0.1316113318918755</v>
+        <v>0.01316113318918755</v>
       </c>
       <c r="H19" t="n">
-        <v>0.2632226637837511</v>
+        <v>0.0263222663783751</v>
       </c>
       <c r="I19" t="n">
         <v>14.1</v>
@@ -1376,7 +1376,7 @@
         <v>0.02500499950009998</v>
       </c>
       <c r="N19" t="n">
-        <v>3.880747661278238e-05</v>
+        <v>3.880747661278237e-06</v>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="n">
@@ -1397,16 +1397,16 @@
         <v>0.1</v>
       </c>
       <c r="E20" t="n">
-        <v>0.01735389</v>
+        <v>0.001735389</v>
       </c>
       <c r="F20" t="n">
         <v>0.5</v>
       </c>
       <c r="G20" t="n">
-        <v>0.09468107529214004</v>
+        <v>0.009468107529214002</v>
       </c>
       <c r="H20" t="n">
-        <v>0.1893621505842801</v>
+        <v>0.018936215058428</v>
       </c>
       <c r="I20" t="n">
         <v>14.1</v>
@@ -1424,7 +1424,7 @@
         <v>0.02500499950009998</v>
       </c>
       <c r="N20" t="n">
-        <v>3.767226321138434e-05</v>
+        <v>3.767226321138433e-06</v>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="n">
@@ -1445,16 +1445,16 @@
         <v>0.1</v>
       </c>
       <c r="E21" t="n">
-        <v>0.01585786500000001</v>
+        <v>0.0015857865</v>
       </c>
       <c r="F21" t="n">
         <v>0.5</v>
       </c>
       <c r="G21" t="n">
-        <v>0.08718316632483276</v>
+        <v>0.008718316632483274</v>
       </c>
       <c r="H21" t="n">
-        <v>0.1743663326496655</v>
+        <v>0.01743663326496655</v>
       </c>
       <c r="I21" t="n">
         <v>14.1</v>
@@ -1472,7 +1472,7 @@
         <v>0.02500499950009998</v>
       </c>
       <c r="N21" t="n">
-        <v>3.593388593339043e-05</v>
+        <v>3.593388593339042e-06</v>
       </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
@@ -1493,16 +1493,16 @@
         <v>0.09</v>
       </c>
       <c r="E22" t="n">
-        <v>0.01436184</v>
+        <v>0.001436184</v>
       </c>
       <c r="F22" t="n">
         <v>0.45</v>
       </c>
       <c r="G22" t="n">
-        <v>0.07775516461876189</v>
+        <v>0.007775516461876189</v>
       </c>
       <c r="H22" t="n">
-        <v>0.1727892547083598</v>
+        <v>0.01727892547083598</v>
       </c>
       <c r="I22" t="n">
         <v>14.1</v>
@@ -1520,7 +1520,7 @@
         <v>0.02500404967200313</v>
       </c>
       <c r="N22" t="n">
-        <v>3.404049516018901e-05</v>
+        <v>3.404049516018901e-06</v>
       </c>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="n">
@@ -1541,16 +1541,16 @@
         <v>0.11</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01121283</v>
+        <v>0.001121283</v>
       </c>
       <c r="F23" t="n">
         <v>0.88</v>
       </c>
       <c r="G23" t="n">
-        <v>0.05730119481576068</v>
+        <v>0.005730119481576068</v>
       </c>
       <c r="H23" t="n">
-        <v>0.06511499410881895</v>
+        <v>0.006511499410881895</v>
       </c>
       <c r="I23" t="n">
         <v>27</v>
@@ -1568,7 +1568,7 @@
         <v>0.04000378107129374</v>
       </c>
       <c r="N23" t="n">
-        <v>1.539639106271662e-05</v>
+        <v>1.539639106271661e-06</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
@@ -1593,16 +1593,16 @@
         <v>0.34</v>
       </c>
       <c r="E24" t="n">
-        <v>0.158474664</v>
+        <v>0.0158474664</v>
       </c>
       <c r="F24" t="n">
         <v>2.72</v>
       </c>
       <c r="G24" t="n">
-        <v>0.2804627333140812</v>
+        <v>0.02804627333140812</v>
       </c>
       <c r="H24" t="n">
-        <v>0.1031112990125298</v>
+        <v>0.01031112990125298</v>
       </c>
       <c r="I24" t="n">
         <v>27</v>
@@ -1620,7 +1620,7 @@
         <v>0.04003610870202048</v>
       </c>
       <c r="N24" t="n">
-        <v>7.808853565740887e-05</v>
+        <v>7.808853565740889e-06</v>
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
@@ -1641,16 +1641,16 @@
         <v>0.2</v>
       </c>
       <c r="E25" t="n">
-        <v>0.05980176000000001</v>
+        <v>0.005980176</v>
       </c>
       <c r="F25" t="n">
         <v>1.6</v>
       </c>
       <c r="G25" t="n">
-        <v>0.224194838732703</v>
+        <v>0.0224194838732703</v>
       </c>
       <c r="H25" t="n">
-        <v>0.1401217742079394</v>
+        <v>0.01401217742079394</v>
       </c>
       <c r="I25" t="n">
         <v>27</v>
@@ -1668,7 +1668,7 @@
         <v>0.04001249804748511</v>
       </c>
       <c r="N25" t="n">
-        <v>4.700597835999596e-05</v>
+        <v>4.700597835999596e-06</v>
       </c>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="n">
@@ -1689,16 +1689,16 @@
         <v>0.16</v>
       </c>
       <c r="E26" t="n">
-        <v>0.043356276</v>
+        <v>0.0043356276</v>
       </c>
       <c r="F26" t="n">
         <v>1.28</v>
       </c>
       <c r="G26" t="n">
-        <v>0.189782809714932</v>
+        <v>0.0189782809714932</v>
       </c>
       <c r="H26" t="n">
-        <v>0.1482678200897906</v>
+        <v>0.01482678200897906</v>
       </c>
       <c r="I26" t="n">
         <v>27</v>
@@ -1716,7 +1716,7 @@
         <v>0.04000799920015995</v>
       </c>
       <c r="N26" t="n">
-        <v>3.939994356867522e-05</v>
+        <v>3.939994356867522e-06</v>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
@@ -1737,16 +1737,16 @@
         <v>0.15</v>
       </c>
       <c r="E27" t="n">
-        <v>0.040366188</v>
+        <v>0.0040366188</v>
       </c>
       <c r="F27" t="n">
         <v>1.2</v>
       </c>
       <c r="G27" t="n">
-        <v>0.1809214774018936</v>
+        <v>0.01809214774018936</v>
       </c>
       <c r="H27" t="n">
-        <v>0.1507678978349113</v>
+        <v>0.01507678978349113</v>
       </c>
       <c r="I27" t="n">
         <v>27</v>
@@ -1764,7 +1764,7 @@
         <v>0.04000703063212765</v>
       </c>
       <c r="N27" t="n">
-        <v>3.780453809449601e-05</v>
+        <v>3.780453809449601e-06</v>
       </c>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="n">
@@ -1785,16 +1785,16 @@
         <v>0.13</v>
       </c>
       <c r="E28" t="n">
-        <v>0.035881056</v>
+        <v>0.0035881056</v>
       </c>
       <c r="F28" t="n">
         <v>1.04</v>
       </c>
       <c r="G28" t="n">
-        <v>0.1660795285807621</v>
+        <v>0.01660795285807621</v>
       </c>
       <c r="H28" t="n">
-        <v>0.159691854404579</v>
+        <v>0.0159691854404579</v>
       </c>
       <c r="I28" t="n">
         <v>27</v>
@@ -1812,7 +1812,7 @@
         <v>0.04000528090140101</v>
       </c>
       <c r="N28" t="n">
-        <v>3.524714175986473e-05</v>
+        <v>3.524714175986473e-06</v>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="n">
@@ -1833,16 +1833,16 @@
         <v>0.12</v>
       </c>
       <c r="E29" t="n">
-        <v>0.028405836</v>
+        <v>0.0028405836</v>
       </c>
       <c r="F29" t="n">
         <v>0.96</v>
       </c>
       <c r="G29" t="n">
-        <v>0.136536535515915</v>
+        <v>0.0136536535515915</v>
       </c>
       <c r="H29" t="n">
-        <v>0.1422255578290781</v>
+        <v>0.01422255578290781</v>
       </c>
       <c r="I29" t="n">
         <v>27</v>
@@ -1860,7 +1860,7 @@
         <v>0.04000449974690348</v>
       </c>
       <c r="N29" t="n">
-        <v>3.044692121693027e-05</v>
+        <v>3.044692121693027e-06</v>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="n">
@@ -1881,16 +1881,16 @@
         <v>0.11</v>
       </c>
       <c r="E30" t="n">
-        <v>0.02242566</v>
+        <v>0.002242566</v>
       </c>
       <c r="F30" t="n">
         <v>0.88</v>
       </c>
       <c r="G30" t="n">
-        <v>0.1117842980832053</v>
+        <v>0.01117842980832053</v>
       </c>
       <c r="H30" t="n">
-        <v>0.1270276114581878</v>
+        <v>0.01270276114581878</v>
       </c>
       <c r="I30" t="n">
         <v>27</v>
@@ -1908,7 +1908,7 @@
         <v>0.04000378107129374</v>
       </c>
       <c r="N30" t="n">
-        <v>2.598094742325615e-05</v>
+        <v>2.598094742325614e-06</v>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="n">
@@ -1929,16 +1929,16 @@
         <v>0.1</v>
       </c>
       <c r="E31" t="n">
-        <v>0.01495044</v>
+        <v>0.001495044</v>
       </c>
       <c r="F31" t="n">
         <v>0.8</v>
       </c>
       <c r="G31" t="n">
-        <v>0.07655815372925405</v>
+        <v>0.007655815372925404</v>
       </c>
       <c r="H31" t="n">
-        <v>0.09569769216156755</v>
+        <v>0.009569769216156754</v>
       </c>
       <c r="I31" t="n">
         <v>27</v>
@@ -1956,7 +1956,7 @@
         <v>0.04000312487793922</v>
       </c>
       <c r="N31" t="n">
-        <v>1.932103097152168e-05</v>
+        <v>1.932103097152168e-06</v>
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="n">
@@ -1977,16 +1977,16 @@
         <v>0.46</v>
       </c>
       <c r="E32" t="n">
-        <v>0.17193006</v>
+        <v>0.017193006</v>
       </c>
       <c r="F32" t="n">
         <v>3.68</v>
       </c>
       <c r="G32" t="n">
-        <v>0.2142532379928102</v>
+        <v>0.02142532379928101</v>
       </c>
       <c r="H32" t="n">
-        <v>0.05822098858500276</v>
+        <v>0.005822098858500275</v>
       </c>
       <c r="I32" t="n">
         <v>27</v>
@@ -2004,7 +2004,7 @@
         <v>0.04006607043372235</v>
       </c>
       <c r="N32" t="n">
-        <v>8.183314021625666e-05</v>
+        <v>8.183314021625664e-06</v>
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="n">
@@ -2025,16 +2025,16 @@
         <v>0.25</v>
       </c>
       <c r="E33" t="n">
-        <v>0.103158036</v>
+        <v>0.0103158036</v>
       </c>
       <c r="F33" t="n">
         <v>2</v>
       </c>
       <c r="G33" t="n">
-        <v>0.3013948910924069</v>
+        <v>0.03013948910924068</v>
       </c>
       <c r="H33" t="n">
-        <v>0.1506974455462034</v>
+        <v>0.01506974455462034</v>
       </c>
       <c r="I33" t="n">
         <v>27</v>
@@ -2052,7 +2052,7 @@
         <v>0.04001952648395531</v>
       </c>
       <c r="N33" t="n">
-        <v>6.212778826576547e-05</v>
+        <v>6.212778826576547e-06</v>
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="n">
@@ -2073,16 +2073,16 @@
         <v>0.23</v>
       </c>
       <c r="E34" t="n">
-        <v>0.08970264000000001</v>
+        <v>0.008970264</v>
       </c>
       <c r="F34" t="n">
         <v>1.84</v>
       </c>
       <c r="G34" t="n">
-        <v>0.2836878825304874</v>
+        <v>0.02836878825304873</v>
       </c>
       <c r="H34" t="n">
-        <v>0.1541781970274388</v>
+        <v>0.01541781970274387</v>
       </c>
       <c r="I34" t="n">
         <v>27</v>
@@ -2100,7 +2100,7 @@
         <v>0.04001652783538322</v>
       </c>
       <c r="N34" t="n">
-        <v>5.787600704126021e-05</v>
+        <v>5.78760070412602e-06</v>
       </c>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="n">
@@ -2121,16 +2121,16 @@
         <v>0.21</v>
       </c>
       <c r="E35" t="n">
-        <v>0.07774228800000001</v>
+        <v>0.007774228799999998</v>
       </c>
       <c r="F35" t="n">
         <v>1.68</v>
       </c>
       <c r="G35" t="n">
-        <v>0.2686580609394681</v>
+        <v>0.0268658060939468</v>
       </c>
       <c r="H35" t="n">
-        <v>0.1599155124639692</v>
+        <v>0.01599155124639691</v>
       </c>
       <c r="I35" t="n">
         <v>27</v>
@@ -2148,7 +2148,7 @@
         <v>0.04001377887678193</v>
       </c>
       <c r="N35" t="n">
-        <v>5.383009871599578e-05</v>
+        <v>5.383009871599576e-06</v>
       </c>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="n">
@@ -2169,16 +2169,16 @@
         <v>0.2</v>
       </c>
       <c r="E36" t="n">
-        <v>0.06578193600000001</v>
+        <v>0.0065781936</v>
       </c>
       <c r="F36" t="n">
         <v>1.6</v>
       </c>
       <c r="G36" t="n">
-        <v>0.2445477221372082</v>
+        <v>0.02445477221372081</v>
       </c>
       <c r="H36" t="n">
-        <v>0.1528423263357551</v>
+        <v>0.01528423263357551</v>
       </c>
       <c r="I36" t="n">
         <v>27</v>
@@ -2196,7 +2196,7 @@
         <v>0.04001249804748511</v>
       </c>
       <c r="N36" t="n">
-        <v>4.9409929335566e-05</v>
+        <v>4.940992933556599e-06</v>
       </c>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="n">
@@ -2217,16 +2217,16 @@
         <v>0.17</v>
       </c>
       <c r="E37" t="n">
-        <v>0.05232654</v>
+        <v>0.005232654</v>
       </c>
       <c r="F37" t="n">
         <v>1.36</v>
       </c>
       <c r="G37" t="n">
-        <v>0.2186369359568574</v>
+        <v>0.02186369359568574</v>
       </c>
       <c r="H37" t="n">
-        <v>0.1607624529094539</v>
+        <v>0.01607624529094539</v>
       </c>
       <c r="I37" t="n">
         <v>27</v>
@@ -2244,7 +2244,7 @@
         <v>0.04000903023068668</v>
       </c>
       <c r="N37" t="n">
-        <v>4.375935236257245e-05</v>
+        <v>4.375935236257245e-06</v>
       </c>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="n">
@@ -2265,16 +2265,16 @@
         <v>0.16</v>
       </c>
       <c r="E38" t="n">
-        <v>0.04485132000000001</v>
+        <v>0.004485132</v>
       </c>
       <c r="F38" t="n">
         <v>1.28</v>
       </c>
       <c r="G38" t="n">
-        <v>0.1925695891349335</v>
+        <v>0.01925695891349334</v>
       </c>
       <c r="H38" t="n">
-        <v>0.1504449915116668</v>
+        <v>0.01504449915116668</v>
       </c>
       <c r="I38" t="n">
         <v>27</v>
@@ -2292,7 +2292,7 @@
         <v>0.04000799920015995</v>
       </c>
       <c r="N38" t="n">
-        <v>4.016844627577722e-05</v>
+        <v>4.016844627577722e-06</v>
       </c>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="n">
@@ -2313,16 +2313,16 @@
         <v>0.15</v>
       </c>
       <c r="E39" t="n">
-        <v>0.040366188</v>
+        <v>0.0040366188</v>
       </c>
       <c r="F39" t="n">
         <v>1.2</v>
       </c>
       <c r="G39" t="n">
-        <v>0.1809214774018936</v>
+        <v>0.01809214774018936</v>
       </c>
       <c r="H39" t="n">
-        <v>0.1507678978349113</v>
+        <v>0.01507678978349113</v>
       </c>
       <c r="I39" t="n">
         <v>27</v>
@@ -2340,7 +2340,7 @@
         <v>0.04000703063212765</v>
       </c>
       <c r="N39" t="n">
-        <v>3.780453809449601e-05</v>
+        <v>3.780453809449601e-06</v>
       </c>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="n">
@@ -2361,16 +2361,16 @@
         <v>0.31</v>
       </c>
       <c r="E40" t="n">
-        <v>0.137544048</v>
+        <v>0.0137544048</v>
       </c>
       <c r="F40" t="n">
         <v>2.48</v>
       </c>
       <c r="G40" t="n">
-        <v>0.2621451382500264</v>
+        <v>0.02621451382500264</v>
       </c>
       <c r="H40" t="n">
-        <v>0.1057036847782365</v>
+        <v>0.01057036847782365</v>
       </c>
       <c r="I40" t="n">
         <v>27</v>
@@ -2388,7 +2388,7 @@
         <v>0.04003001998500625</v>
       </c>
       <c r="N40" t="n">
-        <v>7.220796659648651e-05</v>
+        <v>7.220796659648651e-06</v>
       </c>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="n">
@@ -2409,16 +2409,16 @@
         <v>0.27</v>
       </c>
       <c r="E41" t="n">
-        <v>0.118108476</v>
+        <v>0.0118108476</v>
       </c>
       <c r="F41" t="n">
         <v>2.16</v>
       </c>
       <c r="G41" t="n">
-        <v>0.2795233694646425</v>
+        <v>0.02795233694646424</v>
       </c>
       <c r="H41" t="n">
-        <v>0.1294089673447419</v>
+        <v>0.01294089673447418</v>
       </c>
       <c r="I41" t="n">
         <v>27</v>
@@ -2436,7 +2436,7 @@
         <v>0.0400227747663752</v>
       </c>
       <c r="N41" t="n">
-        <v>6.660931695708943e-05</v>
+        <v>6.660931695708942e-06</v>
       </c>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="n">
@@ -2457,16 +2457,16 @@
         <v>0.35</v>
       </c>
       <c r="E42" t="n">
-        <v>0.168939972</v>
+        <v>0.0168939972</v>
       </c>
       <c r="F42" t="n">
         <v>2.8</v>
       </c>
       <c r="G42" t="n">
-        <v>0.2264493119713559</v>
+        <v>0.02264493119713559</v>
       </c>
       <c r="H42" t="n">
-        <v>0.08087475427548427</v>
+        <v>0.008087475427548424</v>
       </c>
       <c r="I42" t="n">
         <v>27</v>
@@ -2484,7 +2484,7 @@
         <v>0.04003826294933385</v>
       </c>
       <c r="N42" t="n">
-        <v>8.100217518130307e-05</v>
+        <v>8.100217518130305e-06</v>
       </c>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="n">
@@ -2505,16 +2505,16 @@
         <v>0.51</v>
       </c>
       <c r="E43" t="n">
-        <v>0.228329712</v>
+        <v>0.0228329712</v>
       </c>
       <c r="F43" t="n">
         <v>4.335</v>
       </c>
       <c r="G43" t="n">
-        <v>1.128581808083011</v>
+        <v>0.1128581808083011</v>
       </c>
       <c r="H43" t="n">
-        <v>0.2603418242406024</v>
+        <v>0.02603418242406024</v>
       </c>
       <c r="I43" t="n">
         <v>20</v>
@@ -2532,7 +2532,7 @@
         <v>0.04257643127365186</v>
       </c>
       <c r="N43" t="n">
-        <v>0.0001024721135375306</v>
+        <v>1.024721135375306e-05</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -2557,16 +2557,16 @@
         <v>0.43</v>
       </c>
       <c r="E44" t="n">
-        <v>0.198324846</v>
+        <v>0.0198324846</v>
       </c>
       <c r="F44" t="n">
         <v>3.655</v>
       </c>
       <c r="G44" t="n">
-        <v>1.221189523267137</v>
+        <v>0.1221189523267137</v>
       </c>
       <c r="H44" t="n">
-        <v>0.3341147806476436</v>
+        <v>0.03341147806476435</v>
       </c>
       <c r="I44" t="n">
         <v>20</v>
@@ -2584,7 +2584,7 @@
         <v>0.04255434760397578</v>
       </c>
       <c r="N44" t="n">
-        <v>9.469847983134858e-05</v>
+        <v>9.469847983134859e-06</v>
       </c>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="n">
@@ -2605,16 +2605,16 @@
         <v>0.39</v>
       </c>
       <c r="E45" t="n">
-        <v>0.17929737</v>
+        <v>0.017929737</v>
       </c>
       <c r="F45" t="n">
         <v>3.315</v>
       </c>
       <c r="G45" t="n">
-        <v>1.16786574949594</v>
+        <v>0.116786574949594</v>
       </c>
       <c r="H45" t="n">
-        <v>0.3522973603306003</v>
+        <v>0.03522973603306002</v>
       </c>
       <c r="I45" t="n">
         <v>20</v>
@@ -2632,7 +2632,7 @@
         <v>0.04254471177479053</v>
       </c>
       <c r="N45" t="n">
-        <v>8.992349827676397e-05</v>
+        <v>8.992349827676395e-06</v>
       </c>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="n">
@@ -2653,16 +2653,16 @@
         <v>0.34</v>
       </c>
       <c r="E46" t="n">
-        <v>0.147097026</v>
+        <v>0.0147097026</v>
       </c>
       <c r="F46" t="n">
         <v>2.89</v>
       </c>
       <c r="G46" t="n">
-        <v>0.9411822334887189</v>
+        <v>0.09411822334887189</v>
       </c>
       <c r="H46" t="n">
-        <v>0.3256685929026709</v>
+        <v>0.03256685929026709</v>
       </c>
       <c r="I46" t="n">
         <v>20</v>
@@ -2680,7 +2680,7 @@
         <v>0.04253398641086913</v>
       </c>
       <c r="N46" t="n">
-        <v>8.211180969236212e-05</v>
+        <v>8.211180969236214e-06</v>
       </c>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="n">
@@ -2701,16 +2701,16 @@
         <v>0.33</v>
       </c>
       <c r="E47" t="n">
-        <v>0.141242418</v>
+        <v>0.0141242418</v>
       </c>
       <c r="F47" t="n">
         <v>2.805</v>
       </c>
       <c r="G47" t="n">
-        <v>1.041277348352992</v>
+        <v>0.1041277348352991</v>
       </c>
       <c r="H47" t="n">
-        <v>0.3712218710705852</v>
+        <v>0.03712218710705852</v>
       </c>
       <c r="I47" t="n">
         <v>20</v>
@@ -2728,7 +2728,7 @@
         <v>0.04253201735163758</v>
       </c>
       <c r="N47" t="n">
-        <v>8.07235389796304e-05</v>
+        <v>8.072353897963037e-06</v>
       </c>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="n">
@@ -2749,16 +2749,16 @@
         <v>0.27</v>
       </c>
       <c r="E48" t="n">
-        <v>0.1097739</v>
+        <v>0.01097739</v>
       </c>
       <c r="F48" t="n">
         <v>2.295</v>
       </c>
       <c r="G48" t="n">
-        <v>0.8932000334913828</v>
+        <v>0.08932000334913827</v>
       </c>
       <c r="H48" t="n">
-        <v>0.3891939143753302</v>
+        <v>0.03891939143753301</v>
       </c>
       <c r="I48" t="n">
         <v>20</v>
@@ -2776,7 +2776,7 @@
         <v>0.04252143577067924</v>
       </c>
       <c r="N48" t="n">
-        <v>7.334588447922148e-05</v>
+        <v>7.334588447922147e-06</v>
       </c>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="n">
@@ -2797,16 +2797,16 @@
         <v>0.23</v>
       </c>
       <c r="E49" t="n">
-        <v>0.08050086000000001</v>
+        <v>0.008050086</v>
       </c>
       <c r="F49" t="n">
         <v>1.955</v>
       </c>
       <c r="G49" t="n">
-        <v>0.7249826097664934</v>
+        <v>0.07249826097664933</v>
       </c>
       <c r="H49" t="n">
-        <v>0.3708350945097153</v>
+        <v>0.03708350945097152</v>
       </c>
       <c r="I49" t="n">
         <v>20</v>
@@ -2824,7 +2824,7 @@
         <v>0.04251555597660696</v>
       </c>
       <c r="N49" t="n">
-        <v>6.626687471391086e-05</v>
+        <v>6.626687471391086e-06</v>
       </c>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="n">
@@ -2845,16 +2845,16 @@
         <v>0.21</v>
       </c>
       <c r="E50" t="n">
-        <v>0.07171894800000002</v>
+        <v>0.007171894799999999</v>
       </c>
       <c r="F50" t="n">
         <v>1.785</v>
       </c>
       <c r="G50" t="n">
-        <v>0.6691758088751656</v>
+        <v>0.06691758088751655</v>
       </c>
       <c r="H50" t="n">
-        <v>0.3748884083334261</v>
+        <v>0.03748884083334261</v>
       </c>
       <c r="I50" t="n">
         <v>20</v>
@@ -2872,7 +2872,7 @@
         <v>0.04251296860959019</v>
       </c>
       <c r="N50" t="n">
-        <v>6.395944280079029e-05</v>
+        <v>6.395944280079026e-06</v>
       </c>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="n">
@@ -2893,16 +2893,16 @@
         <v>0.19</v>
       </c>
       <c r="E51" t="n">
-        <v>0.060009732</v>
+        <v>0.0060009732</v>
       </c>
       <c r="F51" t="n">
         <v>1.615</v>
       </c>
       <c r="G51" t="n">
-        <v>0.5819173311288515</v>
+        <v>0.05819173311288516</v>
       </c>
       <c r="H51" t="n">
-        <v>0.3603203288723539</v>
+        <v>0.03603203288723539</v>
       </c>
       <c r="I51" t="n">
         <v>20</v>
@@ -2920,7 +2920,7 @@
         <v>0.04251061632110266</v>
       </c>
       <c r="N51" t="n">
-        <v>6.058710823196233e-05</v>
+        <v>6.058710823196233e-06</v>
       </c>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="n">
@@ -2941,16 +2941,16 @@
         <v>0.16</v>
       </c>
       <c r="E52" t="n">
-        <v>0.04903234200000001</v>
+        <v>0.004903234199999999</v>
       </c>
       <c r="F52" t="n">
         <v>1.36</v>
       </c>
       <c r="G52" t="n">
-        <v>0.4857383485435506</v>
+        <v>0.04857383485435504</v>
       </c>
       <c r="H52" t="n">
-        <v>0.3571605503996695</v>
+        <v>0.03571605503996694</v>
       </c>
       <c r="I52" t="n">
         <v>20</v>
@@ -2968,7 +2968,7 @@
         <v>0.04250752874491764</v>
       </c>
       <c r="N52" t="n">
-        <v>5.690443052176958e-05</v>
+        <v>5.690443052176956e-06</v>
       </c>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="n">
@@ -2989,16 +2989,16 @@
         <v>0.15</v>
       </c>
       <c r="E53" t="n">
-        <v>0.04025043</v>
+        <v>0.004025043</v>
       </c>
       <c r="F53" t="n">
         <v>1.275</v>
       </c>
       <c r="G53" t="n">
-        <v>0.4075919672349995</v>
+        <v>0.04075919672349994</v>
       </c>
       <c r="H53" t="n">
-        <v>0.3196799743019604</v>
+        <v>0.03196799743019603</v>
       </c>
       <c r="I53" t="n">
         <v>20</v>
@@ -3016,7 +3016,7 @@
         <v>0.04250661713192429</v>
       </c>
       <c r="N53" t="n">
-        <v>5.333692805140196e-05</v>
+        <v>5.333692805140195e-06</v>
       </c>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="n">
@@ -3037,16 +3037,16 @@
         <v>0.13</v>
       </c>
       <c r="E54" t="n">
-        <v>0.02854121400000001</v>
+        <v>0.0028541214</v>
       </c>
       <c r="F54" t="n">
         <v>1.105</v>
       </c>
       <c r="G54" t="n">
-        <v>0.3018717230306783</v>
+        <v>0.03018717230306783</v>
       </c>
       <c r="H54" t="n">
-        <v>0.2731870796657723</v>
+        <v>0.02731870796657723</v>
       </c>
       <c r="I54" t="n">
         <v>20</v>
@@ -3064,7 +3064,7 @@
         <v>0.04250497029760167</v>
       </c>
       <c r="N54" t="n">
-        <v>4.701737441815477e-05</v>
+        <v>4.701737441815476e-06</v>
       </c>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="n">
@@ -3085,16 +3085,16 @@
         <v>0.1</v>
       </c>
       <c r="E55" t="n">
-        <v>0.013904694</v>
+        <v>0.0013904694</v>
       </c>
       <c r="F55" t="n">
         <v>0.8500000000000001</v>
       </c>
       <c r="G55" t="n">
-        <v>0.1518708285173636</v>
+        <v>0.01518708285173636</v>
       </c>
       <c r="H55" t="n">
-        <v>0.1786715629616042</v>
+        <v>0.01786715629616042</v>
       </c>
       <c r="I55" t="n">
         <v>20</v>
@@ -3112,7 +3112,7 @@
         <v>0.04250294107470682</v>
       </c>
       <c r="N55" t="n">
-        <v>3.343273750263127e-05</v>
+        <v>3.343273750263127e-06</v>
       </c>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="n">
@@ -3133,16 +3133,16 @@
         <v>0.1</v>
       </c>
       <c r="E56" t="n">
-        <v>0.012441042</v>
+        <v>0.0012441042</v>
       </c>
       <c r="F56" t="n">
         <v>0.8500000000000001</v>
       </c>
       <c r="G56" t="n">
-        <v>0.1360147078027032</v>
+        <v>0.01360147078027032</v>
       </c>
       <c r="H56" t="n">
-        <v>0.1600173032972979</v>
+        <v>0.01600173032972978</v>
       </c>
       <c r="I56" t="n">
         <v>20</v>
@@ -3160,7 +3160,7 @@
         <v>0.04250294107470682</v>
       </c>
       <c r="N56" t="n">
-        <v>3.138080119035403e-05</v>
+        <v>3.138080119035403e-06</v>
       </c>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="n">
@@ -3181,16 +3181,16 @@
         <v>0.66</v>
       </c>
       <c r="E57" t="n">
-        <v>0.3241989180000001</v>
+        <v>0.0324198918</v>
       </c>
       <c r="F57" t="n">
         <v>5.61</v>
       </c>
       <c r="G57" t="n">
-        <v>0.8860958170087873</v>
+        <v>0.0886095817008787</v>
       </c>
       <c r="H57" t="n">
-        <v>0.1579493434953275</v>
+        <v>0.01579493434953274</v>
       </c>
       <c r="I57" t="n">
         <v>20</v>
@@ -3208,7 +3208,7 @@
         <v>0.04262792511957391</v>
       </c>
       <c r="N57" t="n">
-        <v>0.0001290114919239752</v>
+        <v>1.290114919239751e-05</v>
       </c>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="n">
@@ -3229,16 +3229,16 @@
         <v>0.57</v>
       </c>
       <c r="E58" t="n">
-        <v>0.283216662</v>
+        <v>0.0283216662</v>
       </c>
       <c r="F58" t="n">
         <v>4.845</v>
       </c>
       <c r="G58" t="n">
-        <v>1.144813448331272</v>
+        <v>0.1144813448331271</v>
       </c>
       <c r="H58" t="n">
-        <v>0.236287605434731</v>
+        <v>0.0236287605434731</v>
       </c>
       <c r="I58" t="n">
         <v>20</v>
@@ -3256,7 +3256,7 @@
         <v>0.0425954516351218</v>
       </c>
       <c r="N58" t="n">
-        <v>0.0001173878385215581</v>
+        <v>1.173878385215581e-05</v>
       </c>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="n">
@@ -3277,16 +3277,16 @@
         <v>0.52</v>
       </c>
       <c r="E59" t="n">
-        <v>0.2524799700000001</v>
+        <v>0.025247997</v>
       </c>
       <c r="F59" t="n">
         <v>4.42</v>
       </c>
       <c r="G59" t="n">
-        <v>1.205647612774469</v>
+        <v>0.1205647612774468</v>
       </c>
       <c r="H59" t="n">
-        <v>0.2727709531163957</v>
+        <v>0.02727709531163956</v>
       </c>
       <c r="I59" t="n">
         <v>20</v>
@@ -3304,7 +3304,7 @@
         <v>0.04257945513977369</v>
       </c>
       <c r="N59" t="n">
-        <v>0.0001089321606644941</v>
+        <v>1.089321606644941e-05</v>
       </c>
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="n">
@@ -3325,16 +3325,16 @@
         <v>0.49</v>
       </c>
       <c r="E60" t="n">
-        <v>0.236379798</v>
+        <v>0.0236379798</v>
       </c>
       <c r="F60" t="n">
         <v>4.165</v>
       </c>
       <c r="G60" t="n">
-        <v>1.242632455002091</v>
+        <v>0.1242632455002091</v>
       </c>
       <c r="H60" t="n">
-        <v>0.2983511296523628</v>
+        <v>0.02983511296523628</v>
       </c>
       <c r="I60" t="n">
         <v>20</v>
@@ -3352,7 +3352,7 @@
         <v>0.04257055907549254</v>
       </c>
       <c r="N60" t="n">
-        <v>0.0001046062385224625</v>
+        <v>1.046062385224625e-05</v>
       </c>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="n">
@@ -3373,16 +3373,16 @@
         <v>0.26</v>
       </c>
       <c r="E61" t="n">
-        <v>0.09074642400000001</v>
+        <v>0.009074642400000001</v>
       </c>
       <c r="F61" t="n">
         <v>2.21</v>
       </c>
       <c r="G61" t="n">
-        <v>0.7925454711586858</v>
+        <v>0.07925454711586857</v>
       </c>
       <c r="H61" t="n">
-        <v>0.358617860252799</v>
+        <v>0.0358617860252799</v>
       </c>
       <c r="I61" t="n">
         <v>20</v>
@@ -3400,7 +3400,7 @@
         <v>0.04251987770443372</v>
       </c>
       <c r="N61" t="n">
-        <v>6.881642970169731e-05</v>
+        <v>6.881642970169731e-06</v>
       </c>
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="n">
@@ -3421,16 +3421,16 @@
         <v>0.22</v>
       </c>
       <c r="E62" t="n">
-        <v>0.079769034</v>
+        <v>0.007976903399999999</v>
       </c>
       <c r="F62" t="n">
         <v>1.87</v>
       </c>
       <c r="G62" t="n">
-        <v>0.6782955689768794</v>
+        <v>0.06782955689768792</v>
       </c>
       <c r="H62" t="n">
-        <v>0.3627249031961922</v>
+        <v>0.03627249031961921</v>
       </c>
       <c r="I62" t="n">
         <v>20</v>
@@ -3448,7 +3448,7 @@
         <v>0.04251423291087351</v>
       </c>
       <c r="N62" t="n">
-        <v>6.607971995364218e-05</v>
+        <v>6.607971995364218e-06</v>
       </c>
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="n">
@@ -3469,16 +3469,16 @@
         <v>0.12</v>
       </c>
       <c r="E63" t="n">
-        <v>0.019455192</v>
+        <v>0.0019455192</v>
       </c>
       <c r="F63" t="n">
         <v>1.08</v>
       </c>
       <c r="G63" t="n">
-        <v>0.2159583518568722</v>
+        <v>0.02159583518568721</v>
       </c>
       <c r="H63" t="n">
-        <v>0.1999614369045113</v>
+        <v>0.01999614369045112</v>
       </c>
       <c r="I63" t="n">
         <v>26.1</v>
@@ -3496,7 +3496,7 @@
         <v>0.04500399982223803</v>
       </c>
       <c r="N63" t="n">
-        <v>2.51915394509764e-05</v>
+        <v>2.519153945097639e-06</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -3521,16 +3521,16 @@
         <v>0.73</v>
       </c>
       <c r="E64" t="n">
-        <v>0.373713912</v>
+        <v>0.0373713912</v>
       </c>
       <c r="F64" t="n">
         <v>6.57</v>
       </c>
       <c r="G64" t="n">
-        <v>0.7827045869890017</v>
+        <v>0.07827045869890016</v>
       </c>
       <c r="H64" t="n">
-        <v>0.1191331182631662</v>
+        <v>0.01191331182631662</v>
       </c>
       <c r="I64" t="n">
         <v>26.1</v>
@@ -3548,7 +3548,7 @@
         <v>0.04514778510624858</v>
       </c>
       <c r="N64" t="n">
-        <v>0.0001423699132220511</v>
+        <v>1.423699132220511e-05</v>
       </c>
       <c r="O64" t="inlineStr"/>
       <c r="P64" t="n">
@@ -3569,16 +3569,16 @@
         <v>0.63</v>
       </c>
       <c r="E65" t="n">
-        <v>0.309831192</v>
+        <v>0.0309831192</v>
       </c>
       <c r="F65" t="n">
         <v>5.67</v>
       </c>
       <c r="G65" t="n">
-        <v>1.116123361480727</v>
+        <v>0.1116123361480727</v>
       </c>
       <c r="H65" t="n">
-        <v>0.1968471537003046</v>
+        <v>0.01968471537003045</v>
       </c>
       <c r="I65" t="n">
         <v>26.1</v>
@@ -3596,7 +3596,7 @@
         <v>0.04511011527362793</v>
       </c>
       <c r="N65" t="n">
-        <v>0.0001229749557030098</v>
+        <v>1.229749557030098e-05</v>
       </c>
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="n">
@@ -3617,16 +3617,16 @@
         <v>0.13</v>
       </c>
       <c r="E66" t="n">
-        <v>0.021342636</v>
+        <v>0.002134263599999999</v>
       </c>
       <c r="F66" t="n">
         <v>1.17</v>
       </c>
       <c r="G66" t="n">
-        <v>0.2378035334921829</v>
+        <v>0.02378035334921829</v>
       </c>
       <c r="H66" t="n">
-        <v>0.2032508833266521</v>
+        <v>0.0203250883326652</v>
       </c>
       <c r="I66" t="n">
         <v>26.1</v>
@@ -3644,7 +3644,7 @@
         <v>0.04500469419960545</v>
       </c>
       <c r="N66" t="n">
-        <v>2.682572308583098e-05</v>
+        <v>2.682572308583097e-06</v>
       </c>
       <c r="O66" t="inlineStr"/>
       <c r="P66" t="n">
@@ -3665,16 +3665,16 @@
         <v>0.26</v>
       </c>
       <c r="E67" t="n">
-        <v>0.106858368</v>
+        <v>0.0106858368</v>
       </c>
       <c r="F67" t="n">
         <v>2.34</v>
       </c>
       <c r="G67" t="n">
-        <v>0.9657127177712319</v>
+        <v>0.09657127177712319</v>
       </c>
       <c r="H67" t="n">
-        <v>0.4126977426372786</v>
+        <v>0.04126977426372786</v>
       </c>
       <c r="I67" t="n">
         <v>26.1</v>
@@ -3692,7 +3692,7 @@
         <v>0.04501877386157913</v>
       </c>
       <c r="N67" t="n">
-        <v>6.439379564635718e-05</v>
+        <v>6.439379564635718e-06</v>
       </c>
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="n">
@@ -3713,16 +3713,16 @@
         <v>0.35</v>
       </c>
       <c r="E68" t="n">
-        <v>0.146204316</v>
+        <v>0.0146204316</v>
       </c>
       <c r="F68" t="n">
         <v>3.15</v>
       </c>
       <c r="G68" t="n">
-        <v>1.146754964654906</v>
+        <v>0.1146754964654906</v>
       </c>
       <c r="H68" t="n">
-        <v>0.3640491951285416</v>
+        <v>0.03640491951285416</v>
       </c>
       <c r="I68" t="n">
         <v>26.1</v>
@@ -3740,7 +3740,7 @@
         <v>0.04503401492205642</v>
       </c>
       <c r="N68" t="n">
-        <v>7.574526815905497e-05</v>
+        <v>7.574526815905496e-06</v>
       </c>
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="n">
@@ -3761,16 +3761,16 @@
         <v>0.41</v>
       </c>
       <c r="E69" t="n">
-        <v>0.185695452</v>
+        <v>0.0185695452</v>
       </c>
       <c r="F69" t="n">
         <v>3.69</v>
       </c>
       <c r="G69" t="n">
-        <v>1.285379427404147</v>
+        <v>0.1285379427404147</v>
       </c>
       <c r="H69" t="n">
-        <v>0.3483413082396062</v>
+        <v>0.03483413082396061</v>
       </c>
       <c r="I69" t="n">
         <v>26.1</v>
@@ -3788,7 +3788,7 @@
         <v>0.04504667024320443</v>
       </c>
       <c r="N69" t="n">
-        <v>8.687437457565096e-05</v>
+        <v>8.687437457565094e-06</v>
       </c>
       <c r="O69" t="inlineStr"/>
       <c r="P69" t="n">
@@ -3809,16 +3809,16 @@
         <v>0.49</v>
       </c>
       <c r="E70" t="n">
-        <v>0.2267836560000001</v>
+        <v>0.0226783656</v>
       </c>
       <c r="F70" t="n">
         <v>4.41</v>
       </c>
       <c r="G70" t="n">
-        <v>1.327553946709679</v>
+        <v>0.1327553946709679</v>
       </c>
       <c r="H70" t="n">
-        <v>0.3010326409772515</v>
+        <v>0.03010326409772515</v>
       </c>
       <c r="I70" t="n">
         <v>26.1</v>
@@ -3836,7 +3836,7 @@
         <v>0.0450666450936832</v>
       </c>
       <c r="N70" t="n">
-        <v>9.857897712811115e-05</v>
+        <v>9.857897712811111e-06</v>
       </c>
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="n">
@@ -3857,16 +3857,16 @@
         <v>0.53</v>
       </c>
       <c r="E71" t="n">
-        <v>0.2520463680000001</v>
+        <v>0.0252046368</v>
       </c>
       <c r="F71" t="n">
         <v>4.77</v>
       </c>
       <c r="G71" t="n">
-        <v>1.375139588053078</v>
+        <v>0.1375139588053078</v>
       </c>
       <c r="H71" t="n">
-        <v>0.2882892218140625</v>
+        <v>0.02882892218140624</v>
       </c>
       <c r="I71" t="n">
         <v>26.1</v>
@@ -3884,7 +3884,7 @@
         <v>0.045077960246666</v>
       </c>
       <c r="N71" t="n">
-        <v>0.0001058923530812395</v>
+        <v>1.058923530812394e-05</v>
       </c>
       <c r="O71" t="inlineStr"/>
       <c r="P71" t="n">
@@ -3905,16 +3905,16 @@
         <v>0.55</v>
       </c>
       <c r="E72" t="n">
-        <v>0.2603220840000001</v>
+        <v>0.0260322084</v>
       </c>
       <c r="F72" t="n">
         <v>4.95</v>
       </c>
       <c r="G72" t="n">
-        <v>1.343960639013872</v>
+        <v>0.1343960639013871</v>
       </c>
       <c r="H72" t="n">
-        <v>0.2715071998007821</v>
+        <v>0.02715071998007821</v>
       </c>
       <c r="I72" t="n">
         <v>26.1</v>
@@ -3932,7 +3932,7 @@
         <v>0.04508394947206822</v>
       </c>
       <c r="N72" t="n">
-        <v>0.000108308969140759</v>
+        <v>1.08308969140759e-05</v>
       </c>
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="n">
@@ -3953,16 +3953,16 @@
         <v>0.58</v>
       </c>
       <c r="E73" t="n">
-        <v>0.266565168</v>
+        <v>0.0266565168</v>
       </c>
       <c r="F73" t="n">
         <v>5.22</v>
       </c>
       <c r="G73" t="n">
-        <v>1.261741688060872</v>
+        <v>0.1261741688060872</v>
       </c>
       <c r="H73" t="n">
-        <v>0.2417129670614697</v>
+        <v>0.02417129670614697</v>
       </c>
       <c r="I73" t="n">
         <v>26.1</v>
@@ -3980,7 +3980,7 @@
         <v>0.04509334762467742</v>
       </c>
       <c r="N73" t="n">
-        <v>0.0001101388183892137</v>
+        <v>1.101388183892137e-05</v>
       </c>
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="n">
@@ -4001,16 +4001,16 @@
         <v>0.61</v>
       </c>
       <c r="E74" t="n">
-        <v>0.2982161520000001</v>
+        <v>0.0298216152</v>
       </c>
       <c r="F74" t="n">
         <v>5.49</v>
       </c>
       <c r="G74" t="n">
-        <v>1.233550335201606</v>
+        <v>0.1233550335201606</v>
       </c>
       <c r="H74" t="n">
-        <v>0.2246904071405476</v>
+        <v>0.02246904071405475</v>
       </c>
       <c r="I74" t="n">
         <v>26.1</v>
@@ -4028,7 +4028,7 @@
         <v>0.04510324267721779</v>
       </c>
       <c r="N74" t="n">
-        <v>0.0001195032481202116</v>
+        <v>1.195032481202116e-05</v>
       </c>
       <c r="O74" t="inlineStr"/>
       <c r="P74" t="n">
@@ -4049,16 +4049,16 @@
         <v>0.64</v>
       </c>
       <c r="E75" t="n">
-        <v>0.316074276</v>
+        <v>0.0316074276</v>
       </c>
       <c r="F75" t="n">
         <v>5.76</v>
       </c>
       <c r="G75" t="n">
-        <v>1.11213381828675</v>
+        <v>0.111213381828675</v>
       </c>
       <c r="H75" t="n">
-        <v>0.1930787878970053</v>
+        <v>0.01930787878970053</v>
       </c>
       <c r="I75" t="n">
         <v>26.1</v>
@@ -4076,7 +4076,7 @@
         <v>0.04511363430272494</v>
       </c>
       <c r="N75" t="n">
-        <v>0.0001248484337708273</v>
+        <v>1.248484337708273e-05</v>
       </c>
       <c r="O75" t="inlineStr"/>
       <c r="P75" t="n">
@@ -4097,16 +4097,16 @@
         <v>0.71</v>
       </c>
       <c r="E76" t="n">
-        <v>0.3446763120000001</v>
+        <v>0.0344676312</v>
       </c>
       <c r="F76" t="n">
         <v>6.39</v>
       </c>
       <c r="G76" t="n">
-        <v>0.7543733568531178</v>
+        <v>0.07543733568531177</v>
       </c>
       <c r="H76" t="n">
-        <v>0.1180552984120685</v>
+        <v>0.01180552984120685</v>
       </c>
       <c r="I76" t="n">
         <v>26.1</v>
@@ -4124,7 +4124,7 @@
         <v>0.04513981058888041</v>
       </c>
       <c r="N76" t="n">
-        <v>0.0001334945501797768</v>
+        <v>1.334945501797767e-05</v>
       </c>
       <c r="O76" t="inlineStr"/>
       <c r="P76" t="n">
@@ -4145,16 +4145,16 @@
         <v>0.23</v>
       </c>
       <c r="E77" t="n">
-        <v>0.07753039200000002</v>
+        <v>0.007753039199999999</v>
       </c>
       <c r="F77" t="n">
         <v>2.07</v>
       </c>
       <c r="G77" t="n">
-        <v>0.7794205117988382</v>
+        <v>0.07794205117988379</v>
       </c>
       <c r="H77" t="n">
-        <v>0.3765316482119991</v>
+        <v>0.03765316482119989</v>
       </c>
       <c r="I77" t="n">
         <v>26.1</v>
@@ -4172,7 +4172,7 @@
         <v>0.04501469204604204</v>
       </c>
       <c r="N77" t="n">
-        <v>5.508256930259359e-05</v>
+        <v>5.508256930259358e-06</v>
       </c>
       <c r="O77" t="inlineStr"/>
       <c r="P77" t="n">
@@ -4193,16 +4193,16 @@
         <v>0.33</v>
       </c>
       <c r="E78" t="n">
-        <v>0.13938048</v>
+        <v>0.013938048</v>
       </c>
       <c r="F78" t="n">
         <v>2.97</v>
       </c>
       <c r="G78" t="n">
-        <v>1.139938988230136</v>
+        <v>0.1139938988230136</v>
       </c>
       <c r="H78" t="n">
-        <v>0.3838178411549278</v>
+        <v>0.03838178411549278</v>
       </c>
       <c r="I78" t="n">
         <v>26.1</v>
@@ -4220,7 +4220,7 @@
         <v>0.04503023983946788</v>
       </c>
       <c r="N78" t="n">
-        <v>7.381377475667859e-05</v>
+        <v>7.381377475667859e-06</v>
       </c>
       <c r="O78" t="inlineStr"/>
       <c r="P78" t="n">
@@ -4293,16 +4293,16 @@
         <v>0.13</v>
       </c>
       <c r="E80" t="n">
-        <v>0.0337609188</v>
+        <v>0.00337609188</v>
       </c>
       <c r="F80" t="n">
         <v>1.2389</v>
       </c>
       <c r="G80" t="n">
-        <v>0.4048073246006572</v>
+        <v>0.04048073246006571</v>
       </c>
       <c r="H80" t="n">
-        <v>0.3267473763828051</v>
+        <v>0.03267473763828051</v>
       </c>
       <c r="I80" t="n">
         <v>25</v>
@@ -4320,7 +4320,7 @@
         <v>0.04765443316208891</v>
       </c>
       <c r="N80" t="n">
-        <v>3.59630163858457e-05</v>
+        <v>3.596301638584569e-06</v>
       </c>
       <c r="O80" t="inlineStr"/>
       <c r="P80" t="n">
@@ -4341,16 +4341,16 @@
         <v>0.16</v>
       </c>
       <c r="E81" t="n">
-        <v>0.048329946</v>
+        <v>0.0048329946</v>
       </c>
       <c r="F81" t="n">
         <v>1.5248</v>
       </c>
       <c r="G81" t="n">
-        <v>0.5572271221183084</v>
+        <v>0.05572271221183083</v>
       </c>
       <c r="H81" t="n">
-        <v>0.3654427610954278</v>
+        <v>0.03654427610954279</v>
       </c>
       <c r="I81" t="n">
         <v>25</v>
@@ -4368,7 +4368,7 @@
         <v>0.04765671516166426</v>
       </c>
       <c r="N81" t="n">
-        <v>4.362385959469624e-05</v>
+        <v>4.362385959469624e-06</v>
       </c>
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="n">
@@ -4389,16 +4389,16 @@
         <v>0.21</v>
       </c>
       <c r="E82" t="n">
-        <v>0.07410591720000001</v>
+        <v>0.00741059172</v>
       </c>
       <c r="F82" t="n">
         <v>2.0013</v>
       </c>
       <c r="G82" t="n">
-        <v>0.7853477744127006</v>
+        <v>0.07853477744127005</v>
       </c>
       <c r="H82" t="n">
-        <v>0.3924188149766156</v>
+        <v>0.03924188149766155</v>
       </c>
       <c r="I82" t="n">
         <v>25</v>
@@ -4416,7 +4416,7 @@
         <v>0.047661567326306</v>
       </c>
       <c r="N82" t="n">
-        <v>5.386302478716731e-05</v>
+        <v>5.38630247871673e-06</v>
       </c>
       <c r="O82" t="inlineStr"/>
       <c r="P82" t="n">
@@ -4437,16 +4437,16 @@
         <v>0.25</v>
       </c>
       <c r="E83" t="n">
-        <v>0.09399824280000001</v>
+        <v>0.009399824279999998</v>
       </c>
       <c r="F83" t="n">
         <v>2.3825</v>
       </c>
       <c r="G83" t="n">
-        <v>0.9351299319309606</v>
+        <v>0.09351299319309604</v>
       </c>
       <c r="H83" t="n">
-        <v>0.3924994467706026</v>
+        <v>0.03924994467706025</v>
       </c>
       <c r="I83" t="n">
         <v>25</v>
@@ -4464,7 +4464,7 @@
         <v>0.04766639277310587</v>
       </c>
       <c r="N83" t="n">
-        <v>6.044625848986537e-05</v>
+        <v>6.044625848986535e-06</v>
       </c>
       <c r="O83" t="inlineStr"/>
       <c r="P83" t="n">
@@ -4485,16 +4485,16 @@
         <v>0.28</v>
       </c>
       <c r="E84" t="n">
-        <v>0.1510135704</v>
+        <v>0.01510135704</v>
       </c>
       <c r="F84" t="n">
         <v>2.6684</v>
       </c>
       <c r="G84" t="n">
-        <v>1.429595011727829</v>
+        <v>0.1429595011727828</v>
       </c>
       <c r="H84" t="n">
-        <v>0.5357498919681565</v>
+        <v>0.05357498919681563</v>
       </c>
       <c r="I84" t="n">
         <v>25</v>
@@ -4512,7 +4512,7 @@
         <v>0.04767056219513254</v>
       </c>
       <c r="N84" t="n">
-        <v>7.745723469299576e-05</v>
+        <v>7.745723469299574e-06</v>
       </c>
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="n">
@@ -4533,16 +4533,16 @@
         <v>0.34</v>
       </c>
       <c r="E85" t="n">
-        <v>0.1361643696</v>
+        <v>0.01361643696</v>
       </c>
       <c r="F85" t="n">
         <v>3.2402</v>
       </c>
       <c r="G85" t="n">
-        <v>1.160690694459536</v>
+        <v>0.1160690694459536</v>
       </c>
       <c r="H85" t="n">
-        <v>0.3582157565766113</v>
+        <v>0.03582157565766114</v>
       </c>
       <c r="I85" t="n">
         <v>25</v>
@@ -4560,7 +4560,7 @@
         <v>0.04768031564492836</v>
       </c>
       <c r="N85" t="n">
-        <v>7.312195408049543e-05</v>
+        <v>7.312195408049542e-06</v>
       </c>
       <c r="O85" t="inlineStr"/>
       <c r="P85" t="n">
@@ -4581,16 +4581,16 @@
         <v>0.38</v>
       </c>
       <c r="E86" t="n">
-        <v>0.1633412088</v>
+        <v>0.01633412088</v>
       </c>
       <c r="F86" t="n">
         <v>3.6214</v>
       </c>
       <c r="G86" t="n">
-        <v>1.289720874540985</v>
+        <v>0.1289720874540985</v>
       </c>
       <c r="H86" t="n">
-        <v>0.3561387514610331</v>
+        <v>0.03561387514610332</v>
       </c>
       <c r="I86" t="n">
         <v>25</v>
@@ -4608,7 +4608,7 @@
         <v>0.04768786533280767</v>
       </c>
       <c r="N86" t="n">
-        <v>8.105294333873128e-05</v>
+        <v>8.105294333873129e-06</v>
       </c>
       <c r="O86" t="inlineStr"/>
       <c r="P86" t="n">
@@ -4629,16 +4629,16 @@
         <v>0.43</v>
       </c>
       <c r="E87" t="n">
-        <v>0.1867357044</v>
+        <v>0.01867357044</v>
       </c>
       <c r="F87" t="n">
         <v>4.0979</v>
       </c>
       <c r="G87" t="n">
-        <v>1.331689863830518</v>
+        <v>0.1331689863830518</v>
       </c>
       <c r="H87" t="n">
-        <v>0.3249688532737545</v>
+        <v>0.03249688532737544</v>
       </c>
       <c r="I87" t="n">
         <v>25</v>
@@ -4656,7 +4656,7 @@
         <v>0.04769848005964131</v>
       </c>
       <c r="N87" t="n">
-        <v>8.790692274016674e-05</v>
+        <v>8.790692274016673e-06</v>
       </c>
       <c r="O87" t="inlineStr"/>
       <c r="P87" t="n">
@@ -4677,16 +4677,16 @@
         <v>0.47</v>
       </c>
       <c r="E88" t="n">
-        <v>0.1986430824</v>
+        <v>0.01986430824</v>
       </c>
       <c r="F88" t="n">
         <v>4.4791</v>
       </c>
       <c r="G88" t="n">
-        <v>1.316757418027514</v>
+        <v>0.1316757418027514</v>
       </c>
       <c r="H88" t="n">
-        <v>0.2939781246293929</v>
+        <v>0.02939781246293929</v>
       </c>
       <c r="I88" t="n">
         <v>25</v>
@@ -4704,7 +4704,7 @@
         <v>0.04770791338970926</v>
       </c>
       <c r="N88" t="n">
-        <v>9.142142005772113e-05</v>
+        <v>9.142142005772111e-06</v>
       </c>
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="n">
@@ -4725,16 +4725,16 @@
         <v>0.52</v>
       </c>
       <c r="E89" t="n">
-        <v>0.2394083412</v>
+        <v>0.02394083412</v>
       </c>
       <c r="F89" t="n">
         <v>4.9556</v>
       </c>
       <c r="G89" t="n">
-        <v>1.388921370669365</v>
+        <v>0.1388921370669364</v>
       </c>
       <c r="H89" t="n">
-        <v>0.2802730992552597</v>
+        <v>0.02802730992552596</v>
       </c>
       <c r="I89" t="n">
         <v>25</v>
@@ -4752,7 +4752,7 @@
         <v>0.04772088117375872</v>
       </c>
       <c r="N89" t="n">
-        <v>0.0001036238152248013</v>
+        <v>1.036238152248013e-05</v>
       </c>
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="n">
@@ -4773,16 +4773,16 @@
         <v>0.57</v>
       </c>
       <c r="E90" t="n">
-        <v>0.252856674</v>
+        <v>0.0252856674</v>
       </c>
       <c r="F90" t="n">
         <v>5.432099999999999</v>
       </c>
       <c r="G90" t="n">
-        <v>1.270996271119279</v>
+        <v>0.1270996271119279</v>
       </c>
       <c r="H90" t="n">
-        <v>0.2339788058245023</v>
+        <v>0.02339788058245023</v>
       </c>
       <c r="I90" t="n">
         <v>25</v>
@@ -4800,7 +4800,7 @@
         <v>0.04773515476040693</v>
       </c>
       <c r="N90" t="n">
-        <v>0.000107710161015348</v>
+        <v>1.07710161015348e-05</v>
       </c>
       <c r="O90" t="inlineStr"/>
       <c r="P90" t="n">
@@ -4821,16 +4821,16 @@
         <v>0.6</v>
       </c>
       <c r="E91" t="n">
-        <v>0.2640636180000001</v>
+        <v>0.0264063618</v>
       </c>
       <c r="F91" t="n">
         <v>5.717999999999999</v>
       </c>
       <c r="G91" t="n">
-        <v>1.194595664240364</v>
+        <v>0.1194595664240364</v>
       </c>
       <c r="H91" t="n">
-        <v>0.2089184442532991</v>
+        <v>0.0208918444253299</v>
       </c>
       <c r="I91" t="n">
         <v>25</v>
@@ -4848,7 +4848,7 @@
         <v>0.04774434521490476</v>
       </c>
       <c r="N91" t="n">
-        <v>0.0001111381613507412</v>
+        <v>1.111381613507411e-05</v>
       </c>
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="n">
@@ -4869,16 +4869,16 @@
         <v>0.61</v>
       </c>
       <c r="E92" t="n">
-        <v>0.2807339472</v>
+        <v>0.02807339472</v>
       </c>
       <c r="F92" t="n">
         <v>5.8133</v>
       </c>
       <c r="G92" t="n">
-        <v>1.170055930141468</v>
+        <v>0.1170055930141468</v>
       </c>
       <c r="H92" t="n">
-        <v>0.2012722429844439</v>
+        <v>0.02012722429844439</v>
       </c>
       <c r="I92" t="n">
         <v>25</v>
@@ -4896,7 +4896,7 @@
         <v>0.04774751302424034</v>
       </c>
       <c r="N92" t="n">
-        <v>0.000116274269038896</v>
+        <v>1.16274269038896e-05</v>
       </c>
       <c r="O92" t="inlineStr"/>
       <c r="P92" t="n">
@@ -4917,16 +4917,16 @@
         <v>0.63</v>
       </c>
       <c r="E93" t="n">
-        <v>0.2922210648</v>
+        <v>0.02922210648</v>
       </c>
       <c r="F93" t="n">
         <v>6.0039</v>
       </c>
       <c r="G93" t="n">
-        <v>1.113887987818505</v>
+        <v>0.1113887987818505</v>
       </c>
       <c r="H93" t="n">
-        <v>0.1855274051563992</v>
+        <v>0.01855274051563992</v>
       </c>
       <c r="I93" t="n">
         <v>25</v>
@@ -4944,7 +4944,7 @@
         <v>0.04775400506763804</v>
       </c>
       <c r="N93" t="n">
-        <v>0.000119838148302019</v>
+        <v>1.19838148302019e-05</v>
       </c>
       <c r="O93" t="inlineStr"/>
       <c r="P93" t="n">
@@ -4965,16 +4965,16 @@
         <v>0.64</v>
       </c>
       <c r="E94" t="n">
-        <v>0.3017469672</v>
+        <v>0.03017469672</v>
       </c>
       <c r="F94" t="n">
         <v>6.0992</v>
       </c>
       <c r="G94" t="n">
-        <v>1.058562095195014</v>
+        <v>0.1058562095195015</v>
       </c>
       <c r="H94" t="n">
-        <v>0.1735575313475561</v>
+        <v>0.01735575313475562</v>
       </c>
       <c r="I94" t="n">
         <v>25</v>
@@ -4992,7 +4992,7 @@
         <v>0.04775732928043611</v>
       </c>
       <c r="N94" t="n">
-        <v>0.000122808196419885</v>
+        <v>1.22808196419885e-05</v>
       </c>
       <c r="O94" t="inlineStr"/>
       <c r="P94" t="n">
@@ -5013,16 +5013,16 @@
         <v>0.65</v>
       </c>
       <c r="E95" t="n">
-        <v>0.3196780776000001</v>
+        <v>0.03196780775999999</v>
       </c>
       <c r="F95" t="n">
         <v>6.1945</v>
       </c>
       <c r="G95" t="n">
-        <v>1.014341283102887</v>
+        <v>0.1014341283102886</v>
       </c>
       <c r="H95" t="n">
-        <v>0.1637486936964867</v>
+        <v>0.01637486936964866</v>
       </c>
       <c r="I95" t="n">
         <v>25</v>
@@ -5040,7 +5040,7 @@
         <v>0.04776070560617797</v>
       </c>
       <c r="N95" t="n">
-        <v>0.0001284331223211134</v>
+        <v>1.284331223211134e-05</v>
       </c>
       <c r="O95" t="inlineStr"/>
       <c r="P95" t="n">
@@ -5061,16 +5061,16 @@
         <v>0.65</v>
       </c>
       <c r="E96" t="n">
-        <v>0.3171565152</v>
+        <v>0.03171565152</v>
       </c>
       <c r="F96" t="n">
         <v>6.1945</v>
       </c>
       <c r="G96" t="n">
-        <v>0.9532002598022065</v>
+        <v>0.09532002598022063</v>
       </c>
       <c r="H96" t="n">
-        <v>0.1538784824928899</v>
+        <v>0.01538784824928899</v>
       </c>
       <c r="I96" t="n">
         <v>25</v>
@@ -5088,7 +5088,7 @@
         <v>0.04776070560617797</v>
       </c>
       <c r="N96" t="n">
-        <v>0.0001276395036888439</v>
+        <v>1.276395036888439e-05</v>
       </c>
       <c r="O96" t="inlineStr"/>
       <c r="P96" t="n">
@@ -5109,16 +5109,16 @@
         <v>0.67</v>
       </c>
       <c r="E97" t="n">
-        <v>0.3196780776000001</v>
+        <v>0.03196780775999999</v>
       </c>
       <c r="F97" t="n">
         <v>6.3851</v>
       </c>
       <c r="G97" t="n">
-        <v>0.8670441990879461</v>
+        <v>0.08670441990879457</v>
       </c>
       <c r="H97" t="n">
-        <v>0.1357917963834468</v>
+        <v>0.01357917963834467</v>
       </c>
       <c r="I97" t="n">
         <v>25</v>
@@ -5136,7 +5136,7 @@
         <v>0.04776761455212097</v>
       </c>
       <c r="N97" t="n">
-        <v>0.0001284331223211134</v>
+        <v>1.284331223211134e-05</v>
       </c>
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="n">
@@ -5157,16 +5157,16 @@
         <v>0.67</v>
       </c>
       <c r="E98" t="n">
-        <v>0.3219194664</v>
+        <v>0.03219194664</v>
       </c>
       <c r="F98" t="n">
         <v>6.3851</v>
       </c>
       <c r="G98" t="n">
-        <v>0.7180512797897483</v>
+        <v>0.07180512797897483</v>
       </c>
       <c r="H98" t="n">
-        <v>0.1124573271819937</v>
+        <v>0.01124573271819938</v>
       </c>
       <c r="I98" t="n">
         <v>25</v>
@@ -5184,7 +5184,7 @@
         <v>0.04776761455212097</v>
       </c>
       <c r="N98" t="n">
-        <v>0.0001291392592826697</v>
+        <v>1.291392592826697e-05</v>
       </c>
       <c r="O98" t="inlineStr"/>
       <c r="P98" t="n">
@@ -5205,16 +5205,16 @@
         <v>0.8</v>
       </c>
       <c r="E99" t="n">
-        <v>0.373925808</v>
+        <v>0.0373925808</v>
       </c>
       <c r="F99" t="n">
         <v>8</v>
       </c>
       <c r="G99" t="n">
-        <v>0.8223057999802993</v>
+        <v>0.08223057999802992</v>
       </c>
       <c r="H99" t="n">
-        <v>0.1027882249975374</v>
+        <v>0.01027882249975374</v>
       </c>
       <c r="I99" t="n">
         <v>26.1</v>
@@ -5232,7 +5232,7 @@
         <v>0.0501597448159378</v>
       </c>
       <c r="N99" t="n">
-        <v>0.0001444780074480226</v>
+        <v>1.444780074480226e-05</v>
       </c>
       <c r="O99" t="inlineStr">
         <is>
@@ -5257,16 +5257,16 @@
         <v>0.63</v>
       </c>
       <c r="E100" t="n">
-        <v>0.289167408</v>
+        <v>0.0289167408</v>
       </c>
       <c r="F100" t="n">
         <v>6.3</v>
       </c>
       <c r="G100" t="n">
-        <v>1.362669306945604</v>
+        <v>0.1362669306945604</v>
       </c>
       <c r="H100" t="n">
-        <v>0.2162967153881911</v>
+        <v>0.02162967153881911</v>
       </c>
       <c r="I100" t="n">
         <v>26.1</v>
@@ -5284,7 +5284,7 @@
         <v>0.05009912673889635</v>
       </c>
       <c r="N100" t="n">
-        <v>0.0001177563481303008</v>
+        <v>1.177563481303008e-05</v>
       </c>
       <c r="O100" t="inlineStr"/>
       <c r="P100" t="n">
@@ -5305,16 +5305,16 @@
         <v>0.57</v>
       </c>
       <c r="E101" t="n">
-        <v>0.248200848</v>
+        <v>0.0248200848</v>
       </c>
       <c r="F101" t="n">
         <v>5.699999999999999</v>
       </c>
       <c r="G101" t="n">
-        <v>1.429534261267855</v>
+        <v>0.1429534261267854</v>
       </c>
       <c r="H101" t="n">
-        <v>0.250795484432957</v>
+        <v>0.02507954844329569</v>
       </c>
       <c r="I101" t="n">
         <v>26.1</v>
@@ -5332,7 +5332,7 @@
         <v>0.05008115913195301</v>
       </c>
       <c r="N101" t="n">
-        <v>0.0001051491741838504</v>
+        <v>1.051491741838504e-05</v>
       </c>
       <c r="O101" t="inlineStr"/>
       <c r="P101" t="n">
@@ -5353,16 +5353,16 @@
         <v>0.52</v>
       </c>
       <c r="E102" t="n">
-        <v>0.225598608</v>
+        <v>0.0225598608</v>
       </c>
       <c r="F102" t="n">
         <v>5.2</v>
       </c>
       <c r="G102" t="n">
-        <v>1.441102490090863</v>
+        <v>0.1441102490090863</v>
       </c>
       <c r="H102" t="n">
-        <v>0.277135094248243</v>
+        <v>0.02771350942482428</v>
       </c>
       <c r="I102" t="n">
         <v>26.1</v>
@@ -5380,7 +5380,7 @@
         <v>0.05006755436407894</v>
       </c>
       <c r="N102" t="n">
-        <v>9.828835796959466e-05</v>
+        <v>9.828835796959464e-06</v>
       </c>
       <c r="O102" t="inlineStr"/>
       <c r="P102" t="n">
@@ -5401,16 +5401,16 @@
         <v>0.5</v>
       </c>
       <c r="E103" t="n">
-        <v>0.3569741280000001</v>
+        <v>0.03569741279999999</v>
       </c>
       <c r="F103" t="n">
         <v>5</v>
       </c>
       <c r="G103" t="n">
-        <v>2.429845812433916</v>
+        <v>0.2429845812433915</v>
       </c>
       <c r="H103" t="n">
-        <v>0.4859691624867832</v>
+        <v>0.0485969162486783</v>
       </c>
       <c r="I103" t="n">
         <v>26.1</v>
@@ -5428,7 +5428,7 @@
         <v>0.05006246098625197</v>
       </c>
       <c r="N103" t="n">
-        <v>0.000139072715111594</v>
+        <v>1.390727151115939e-05</v>
       </c>
       <c r="O103" t="inlineStr"/>
       <c r="P103" t="n">
@@ -5449,16 +5449,16 @@
         <v>0.49</v>
       </c>
       <c r="E104" t="n">
-        <v>0.204409008</v>
+        <v>0.0204409008</v>
       </c>
       <c r="F104" t="n">
         <v>4.9</v>
       </c>
       <c r="G104" t="n">
-        <v>1.434179304554842</v>
+        <v>0.1434179304554843</v>
       </c>
       <c r="H104" t="n">
-        <v>0.2926896539907841</v>
+        <v>0.02926896539907842</v>
       </c>
       <c r="I104" t="n">
         <v>26.1</v>
@@ -5476,7 +5476,7 @@
         <v>0.05005998901318298</v>
       </c>
       <c r="N104" t="n">
-        <v>9.191496572416854e-05</v>
+        <v>9.191496572416855e-06</v>
       </c>
       <c r="O104" t="inlineStr"/>
       <c r="P104" t="n">
@@ -5497,16 +5497,16 @@
         <v>0.48</v>
       </c>
       <c r="E105" t="n">
-        <v>0.198758448</v>
+        <v>0.0198758448</v>
       </c>
       <c r="F105" t="n">
         <v>4.8</v>
       </c>
       <c r="G105" t="n">
-        <v>1.43616158417413</v>
+        <v>0.143616158417413</v>
       </c>
       <c r="H105" t="n">
-        <v>0.2992003300362772</v>
+        <v>0.02992003300362772</v>
       </c>
       <c r="I105" t="n">
         <v>26.1</v>
@@ -5524,7 +5524,7 @@
         <v>0.05005756686056565</v>
       </c>
       <c r="N105" t="n">
-        <v>9.022400269454443e-05</v>
+        <v>9.022400269454442e-06</v>
       </c>
       <c r="O105" t="inlineStr"/>
       <c r="P105" t="n">
@@ -5545,16 +5545,16 @@
         <v>0.47</v>
       </c>
       <c r="E106" t="n">
-        <v>0.191695248</v>
+        <v>0.0191695248</v>
       </c>
       <c r="F106" t="n">
         <v>4.699999999999999</v>
       </c>
       <c r="G106" t="n">
-        <v>1.425273839399534</v>
+        <v>0.1425273839399534</v>
       </c>
       <c r="H106" t="n">
-        <v>0.3032497530637306</v>
+        <v>0.03032497530637307</v>
       </c>
       <c r="I106" t="n">
         <v>26.1</v>
@@ -5572,7 +5572,7 @@
         <v>0.05005519453563236</v>
       </c>
       <c r="N106" t="n">
-        <v>8.811470007620376e-05</v>
+        <v>8.811470007620376e-06</v>
       </c>
       <c r="O106" t="inlineStr"/>
       <c r="P106" t="n">
@@ -5593,16 +5593,16 @@
         <v>0.45</v>
       </c>
       <c r="E107" t="n">
-        <v>0.184632048</v>
+        <v>0.0184632048</v>
       </c>
       <c r="F107" t="n">
         <v>4.5</v>
       </c>
       <c r="G107" t="n">
-        <v>1.392092845473692</v>
+        <v>0.1392092845473691</v>
       </c>
       <c r="H107" t="n">
-        <v>0.3093539656608204</v>
+        <v>0.03093539656608203</v>
       </c>
       <c r="I107" t="n">
         <v>26.1</v>
@@ -5620,7 +5620,7 @@
         <v>0.05005059939701022</v>
       </c>
       <c r="N107" t="n">
-        <v>8.60096397401439e-05</v>
+        <v>8.600963974014387e-06</v>
       </c>
       <c r="O107" t="inlineStr"/>
       <c r="P107" t="n">
@@ -5641,16 +5641,16 @@
         <v>0.44</v>
       </c>
       <c r="E108" t="n">
-        <v>0.174743568</v>
+        <v>0.0174743568</v>
       </c>
       <c r="F108" t="n">
         <v>4.4</v>
       </c>
       <c r="G108" t="n">
-        <v>1.390731877376867</v>
+        <v>0.1390731877376867</v>
       </c>
       <c r="H108" t="n">
-        <v>0.3160754266765607</v>
+        <v>0.03160754266765606</v>
       </c>
       <c r="I108" t="n">
         <v>26.1</v>
@@ -5668,7 +5668,7 @@
         <v>0.05004837659704858</v>
       </c>
       <c r="N108" t="n">
-        <v>8.306797879109175e-05</v>
+        <v>8.306797879109174e-06</v>
       </c>
       <c r="O108" t="inlineStr"/>
       <c r="P108" t="n">
@@ -5689,16 +5689,16 @@
         <v>0.43</v>
       </c>
       <c r="E109" t="n">
-        <v>0.171918288</v>
+        <v>0.0171918288</v>
       </c>
       <c r="F109" t="n">
         <v>4.3</v>
       </c>
       <c r="G109" t="n">
-        <v>1.386249558536238</v>
+        <v>0.1386249558536238</v>
       </c>
       <c r="H109" t="n">
-        <v>0.3223836182642414</v>
+        <v>0.03223836182642414</v>
       </c>
       <c r="I109" t="n">
         <v>26.1</v>
@@ -5716,7 +5716,7 @@
         <v>0.0500462036522252</v>
       </c>
       <c r="N109" t="n">
-        <v>8.222829300503519e-05</v>
+        <v>8.222829300503518e-06</v>
       </c>
       <c r="O109" t="inlineStr"/>
       <c r="P109" t="n">
@@ -5737,16 +5737,16 @@
         <v>0.42</v>
       </c>
       <c r="E110" t="n">
-        <v>0.166267728</v>
+        <v>0.0166267728</v>
       </c>
       <c r="F110" t="n">
         <v>4.2</v>
       </c>
       <c r="G110" t="n">
-        <v>1.358098229316052</v>
+        <v>0.1358098229316052</v>
       </c>
       <c r="H110" t="n">
-        <v>0.3233567212657266</v>
+        <v>0.03233567212657266</v>
       </c>
       <c r="I110" t="n">
         <v>26.1</v>
@@ -5764,7 +5764,7 @@
         <v>0.05004408056903435</v>
       </c>
       <c r="N110" t="n">
-        <v>8.054940879112903e-05</v>
+        <v>8.054940879112901e-06</v>
       </c>
       <c r="O110" t="inlineStr"/>
       <c r="P110" t="n">
@@ -5785,16 +5785,16 @@
         <v>0.39</v>
       </c>
       <c r="E111" t="n">
-        <v>0.146490768</v>
+        <v>0.0146490768</v>
       </c>
       <c r="F111" t="n">
         <v>3.9</v>
       </c>
       <c r="G111" t="n">
-        <v>1.257919142884573</v>
+        <v>0.1257919142884573</v>
       </c>
       <c r="H111" t="n">
-        <v>0.3225433699704034</v>
+        <v>0.03225433699704033</v>
       </c>
       <c r="I111" t="n">
         <v>26.1</v>
@@ -5812,7 +5812,7 @@
         <v>0.05003801055197939</v>
       </c>
       <c r="N111" t="n">
-        <v>7.466611576101879e-05</v>
+        <v>7.466611576101878e-06</v>
       </c>
       <c r="O111" t="inlineStr"/>
       <c r="P111" t="n">
@@ -5833,16 +5833,16 @@
         <v>0.28</v>
       </c>
       <c r="E112" t="n">
-        <v>0.08292196800000001</v>
+        <v>0.0082921968</v>
       </c>
       <c r="F112" t="n">
         <v>2.8</v>
       </c>
       <c r="G112" t="n">
-        <v>0.8509896819340259</v>
+        <v>0.0850989681934026</v>
       </c>
       <c r="H112" t="n">
-        <v>0.3039248864050092</v>
+        <v>0.03039248864050093</v>
       </c>
       <c r="I112" t="n">
         <v>26.1</v>
@@ -5860,7 +5860,7 @@
         <v>0.05001959615990517</v>
       </c>
       <c r="N112" t="n">
-        <v>5.476492133277181e-05</v>
+        <v>5.476492133277181e-06</v>
       </c>
       <c r="O112" t="inlineStr"/>
       <c r="P112" t="n">
@@ -5881,16 +5881,16 @@
         <v>0.17</v>
       </c>
       <c r="E113" t="n">
-        <v>0.029241648</v>
+        <v>0.0029241648</v>
       </c>
       <c r="F113" t="n">
         <v>1.7</v>
       </c>
       <c r="G113" t="n">
-        <v>0.3552126732712136</v>
+        <v>0.03552126732712135</v>
       </c>
       <c r="H113" t="n">
-        <v>0.208948631336008</v>
+        <v>0.02089486313360079</v>
       </c>
       <c r="I113" t="n">
         <v>26.1</v>
@@ -5908,7 +5908,7 @@
         <v>0.05000722447806917</v>
       </c>
       <c r="N113" t="n">
-        <v>3.041317032620011e-05</v>
+        <v>3.04131703262001e-06</v>
       </c>
       <c r="O113" t="inlineStr"/>
       <c r="P113" t="n">
@@ -5929,16 +5929,16 @@
         <v>0.13</v>
       </c>
       <c r="E114" t="n">
-        <v>0.012289968</v>
+        <v>0.0012289968</v>
       </c>
       <c r="F114" t="n">
         <v>1.3</v>
       </c>
       <c r="G114" t="n">
-        <v>0.155727295166003</v>
+        <v>0.0155727295166003</v>
       </c>
       <c r="H114" t="n">
-        <v>0.1197902270507716</v>
+        <v>0.01197902270507716</v>
       </c>
       <c r="I114" t="n">
         <v>26.1</v>
@@ -5956,7 +5956,7 @@
         <v>0.05000422482150884</v>
       </c>
       <c r="N114" t="n">
-        <v>1.632401443759565e-05</v>
+        <v>1.632401443759565e-06</v>
       </c>
       <c r="O114" t="inlineStr"/>
       <c r="P114" t="n">
@@ -5977,16 +5977,16 @@
         <v>0.12</v>
       </c>
       <c r="E115" t="n">
-        <v>0.003814128</v>
+        <v>0.0003814127999999999</v>
       </c>
       <c r="F115" t="n">
         <v>1.2</v>
       </c>
       <c r="G115" t="n">
-        <v>0.04912798966906963</v>
+        <v>0.004912798966906962</v>
       </c>
       <c r="H115" t="n">
-        <v>0.04093999139089136</v>
+        <v>0.004093999139089135</v>
       </c>
       <c r="I115" t="n">
         <v>26.1</v>
@@ -6004,7 +6004,7 @@
         <v>0.05000359987040934</v>
       </c>
       <c r="N115" t="n">
-        <v>5.928788559003941e-06</v>
+        <v>5.928788559003939e-07</v>
       </c>
       <c r="O115" t="inlineStr"/>
       <c r="P115" t="n">
@@ -6025,16 +6025,16 @@
         <v>0.11</v>
       </c>
       <c r="E116" t="n">
-        <v>-0.0004237920000000011</v>
+        <v>-4.23792000000001e-05</v>
       </c>
       <c r="F116" t="n">
         <v>1.1</v>
       </c>
       <c r="G116" t="n">
-        <v>-0.0055030449132472</v>
+        <v>-0.0005503044913247199</v>
       </c>
       <c r="H116" t="n">
-        <v>-0.005002768102951999</v>
+        <v>-0.0005002768102951999</v>
       </c>
       <c r="I116" t="n">
         <v>26.1</v>
@@ -6052,7 +6052,7 @@
         <v>0.05000302490849928</v>
       </c>
       <c r="N116" t="n">
-        <v>-7.21485318561648e-07</v>
+        <v>-7.214853185616478e-08</v>
       </c>
       <c r="O116" t="inlineStr"/>
       <c r="P116" t="n">
@@ -6073,16 +6073,16 @@
         <v>0.1</v>
       </c>
       <c r="E117" t="n">
-        <v>-0.006074352000000002</v>
+        <v>-0.0006074352000000001</v>
       </c>
       <c r="F117" t="n">
         <v>1</v>
       </c>
       <c r="G117" t="n">
-        <v>-0.07951308174382697</v>
+        <v>-0.007951308174382696</v>
       </c>
       <c r="H117" t="n">
-        <v>-0.07951308174382697</v>
+        <v>-0.007951308174382696</v>
       </c>
       <c r="I117" t="n">
         <v>26.1</v>
@@ -6100,7 +6100,7 @@
         <v>0.05000249993750312</v>
       </c>
       <c r="N117" t="n">
-        <v>-1.187032846924243e-05</v>
+        <v>-1.187032846924242e-06</v>
       </c>
       <c r="O117" t="inlineStr"/>
       <c r="P117" t="n">
@@ -6121,16 +6121,16 @@
         <v>0.24</v>
       </c>
       <c r="E118" t="n">
-        <v>0.07020820800000002</v>
+        <v>0.0070208208</v>
       </c>
       <c r="F118" t="n">
         <v>2.4</v>
       </c>
       <c r="G118" t="n">
-        <v>0.7719795666607647</v>
+        <v>0.07719795666607646</v>
       </c>
       <c r="H118" t="n">
-        <v>0.3216581527753187</v>
+        <v>0.03216581527753186</v>
       </c>
       <c r="I118" t="n">
         <v>26.1</v>
@@ -6148,7 +6148,7 @@
         <v>0.05001439792699698</v>
       </c>
       <c r="N118" t="n">
-        <v>5.019706544649201e-05</v>
+        <v>5.0197065446492e-06</v>
       </c>
       <c r="O118" t="inlineStr"/>
       <c r="P118" t="n">
@@ -6169,16 +6169,16 @@
         <v>0.11</v>
       </c>
       <c r="E119" t="n">
-        <v>0.025461855</v>
+        <v>0.0025461855</v>
       </c>
       <c r="F119" t="n">
         <v>1.155</v>
       </c>
       <c r="G119" t="n">
-        <v>0.3412939802230124</v>
+        <v>0.03412939802230124</v>
       </c>
       <c r="H119" t="n">
-        <v>0.2954926235697077</v>
+        <v>0.02954926235697077</v>
       </c>
       <c r="I119" t="n">
         <v>26.1</v>
@@ -6196,7 +6196,7 @@
         <v>0.05250288087333875</v>
       </c>
       <c r="N119" t="n">
-        <v>3.340468633674301e-05</v>
+        <v>3.340468633674301e-06</v>
       </c>
       <c r="O119" t="inlineStr">
         <is>
@@ -6221,16 +6221,16 @@
         <v>0.52</v>
       </c>
       <c r="E120" t="n">
-        <v>-0.002987145000000003</v>
+        <v>-0.0002987145000000002</v>
       </c>
       <c r="F120" t="n">
         <v>5.46</v>
       </c>
       <c r="G120" t="n">
-        <v>-0.0224286987614259</v>
+        <v>-0.00224286987614259</v>
       </c>
       <c r="H120" t="n">
-        <v>-0.00410782028597544</v>
+        <v>-0.0004107820285975439</v>
       </c>
       <c r="I120" t="n">
         <v>26.1</v>
@@ -6248,7 +6248,7 @@
         <v>0.05256434152541056</v>
       </c>
       <c r="N120" t="n">
-        <v>-7.72829777550904e-06</v>
+        <v>-7.728297775509037e-07</v>
       </c>
       <c r="O120" t="inlineStr"/>
       <c r="P120" t="n">
@@ -6269,16 +6269,16 @@
         <v>0.58</v>
       </c>
       <c r="E121" t="n">
-        <v>0.0005689799999999981</v>
+        <v>5.689799999999979e-05</v>
       </c>
       <c r="F121" t="n">
         <v>6.09</v>
       </c>
       <c r="G121" t="n">
-        <v>0.003831215595031359</v>
+        <v>0.0003831215595031358</v>
       </c>
       <c r="H121" t="n">
-        <v>0.0006290994408918489</v>
+        <v>6.290994408918487e-05</v>
       </c>
       <c r="I121" t="n">
         <v>26.1</v>
@@ -6296,7 +6296,7 @@
         <v>0.05258003423353774</v>
       </c>
       <c r="N121" t="n">
-        <v>1.307935814540861e-06</v>
+        <v>1.307935814540861e-07</v>
       </c>
       <c r="O121" t="inlineStr"/>
       <c r="P121" t="n">
@@ -6317,16 +6317,16 @@
         <v>0.67</v>
       </c>
       <c r="E122" t="n">
-        <v>0.004836329999999999</v>
+        <v>0.0004836329999999997</v>
       </c>
       <c r="F122" t="n">
         <v>7.035</v>
       </c>
       <c r="G122" t="n">
-        <v>0.02547490245187656</v>
+        <v>0.002547490245187655</v>
       </c>
       <c r="H122" t="n">
-        <v>0.003621165949094039</v>
+        <v>0.0003621165949094036</v>
       </c>
       <c r="I122" t="n">
         <v>26.1</v>
@@ -6344,7 +6344,7 @@
         <v>0.05260677237770817</v>
       </c>
       <c r="N122" t="n">
-        <v>9.815374407815523e-06</v>
+        <v>9.815374407815519e-07</v>
       </c>
       <c r="O122" t="inlineStr"/>
       <c r="P122" t="n">
@@ -6365,16 +6365,16 @@
         <v>0.73</v>
       </c>
       <c r="E123" t="n">
-        <v>0.007681229999999999</v>
+        <v>0.0007681229999999997</v>
       </c>
       <c r="F123" t="n">
         <v>7.665</v>
       </c>
       <c r="G123" t="n">
-        <v>0.03314031281425271</v>
+        <v>0.00331403128142527</v>
       </c>
       <c r="H123" t="n">
-        <v>0.004323589408252147</v>
+        <v>0.0004323589408252145</v>
       </c>
       <c r="I123" t="n">
         <v>26.1</v>
@@ -6392,7 +6392,7 @@
         <v>0.05262672800013317</v>
       </c>
       <c r="N123" t="n">
-        <v>1.446900176031505e-05</v>
+        <v>1.446900176031504e-06</v>
       </c>
       <c r="O123" t="inlineStr"/>
       <c r="P123" t="n">
@@ -6413,16 +6413,16 @@
         <v>0.23</v>
       </c>
       <c r="E124" t="n">
-        <v>0.083782305</v>
+        <v>0.008378230499999998</v>
       </c>
       <c r="F124" t="n">
         <v>2.415</v>
       </c>
       <c r="G124" t="n">
-        <v>1.007216450747882</v>
+        <v>0.1007216450747882</v>
       </c>
       <c r="H124" t="n">
-        <v>0.4170668533117525</v>
+        <v>0.04170668533117523</v>
       </c>
       <c r="I124" t="n">
         <v>26.1</v>
@@ -6440,7 +6440,7 @@
         <v>0.05251259372760023</v>
       </c>
       <c r="N124" t="n">
-        <v>5.952045253191382e-05</v>
+        <v>5.952045253191382e-06</v>
       </c>
       <c r="O124" t="inlineStr"/>
       <c r="P124" t="n">
@@ -6461,16 +6461,16 @@
         <v>0.29</v>
       </c>
       <c r="E125" t="n">
-        <v>0.11863233</v>
+        <v>0.011863233</v>
       </c>
       <c r="F125" t="n">
         <v>3.045</v>
       </c>
       <c r="G125" t="n">
-        <v>1.269645781490591</v>
+        <v>0.1269645781490591</v>
       </c>
       <c r="H125" t="n">
-        <v>0.4169608477801614</v>
+        <v>0.04169608477801613</v>
       </c>
       <c r="I125" t="n">
         <v>26.1</v>
@@ -6488,7 +6488,7 @@
         <v>0.05252001999238005</v>
       </c>
       <c r="N125" t="n">
-        <v>6.974768222532195e-05</v>
+        <v>6.974768222532194e-06</v>
       </c>
       <c r="O125" t="inlineStr"/>
       <c r="P125" t="n">
@@ -6509,16 +6509,16 @@
         <v>0.35</v>
       </c>
       <c r="E126" t="n">
-        <v>0.14992623</v>
+        <v>0.014992623</v>
       </c>
       <c r="F126" t="n">
         <v>3.675</v>
       </c>
       <c r="G126" t="n">
-        <v>1.466402237756728</v>
+        <v>0.1466402237756728</v>
       </c>
       <c r="H126" t="n">
-        <v>0.3990210170766607</v>
+        <v>0.03990210170766607</v>
       </c>
       <c r="I126" t="n">
         <v>26.1</v>
@@ -6536,7 +6536,7 @@
         <v>0.05252915856931273</v>
       </c>
       <c r="N126" t="n">
-        <v>7.846548979237317e-05</v>
+        <v>7.846548979237314e-06</v>
       </c>
       <c r="O126" t="inlineStr"/>
       <c r="P126" t="n">
@@ -6557,16 +6557,16 @@
         <v>0.41</v>
       </c>
       <c r="E127" t="n">
-        <v>0.1826425800000001</v>
+        <v>0.018264258</v>
       </c>
       <c r="F127" t="n">
         <v>4.305</v>
       </c>
       <c r="G127" t="n">
-        <v>1.673550047052001</v>
+        <v>0.1673550047052001</v>
       </c>
       <c r="H127" t="n">
-        <v>0.3887456555289202</v>
+        <v>0.03887456555289201</v>
       </c>
       <c r="I127" t="n">
         <v>26.1</v>
@@ -6584,7 +6584,7 @@
         <v>0.05254000856490224</v>
       </c>
       <c r="N127" t="n">
-        <v>8.759557469632588e-05</v>
+        <v>8.759557469632585e-06</v>
       </c>
       <c r="O127" t="inlineStr"/>
       <c r="P127" t="n">
@@ -6605,16 +6605,16 @@
         <v>0.44</v>
       </c>
       <c r="E128" t="n">
-        <v>0.19828953</v>
+        <v>0.019828953</v>
       </c>
       <c r="F128" t="n">
         <v>4.62</v>
       </c>
       <c r="G128" t="n">
-        <v>1.758781187766039</v>
+        <v>0.1758781187766039</v>
       </c>
       <c r="H128" t="n">
-        <v>0.3806885687805279</v>
+        <v>0.03806885687805279</v>
       </c>
       <c r="I128" t="n">
         <v>26.1</v>
@@ -6632,7 +6632,7 @@
         <v>0.05254607501992894</v>
       </c>
       <c r="N128" t="n">
-        <v>9.201851210681665e-05</v>
+        <v>9.201851210681665e-06</v>
       </c>
       <c r="O128" t="inlineStr"/>
       <c r="P128" t="n">
@@ -6653,16 +6653,16 @@
         <v>0.6</v>
       </c>
       <c r="E129" t="n">
-        <v>0.297149805</v>
+        <v>0.0297149805</v>
       </c>
       <c r="F129" t="n">
         <v>6.3</v>
       </c>
       <c r="G129" t="n">
-        <v>1.829706343031134</v>
+        <v>0.1829706343031133</v>
       </c>
       <c r="H129" t="n">
-        <v>0.2904295782589102</v>
+        <v>0.02904295782589101</v>
       </c>
       <c r="I129" t="n">
         <v>26.1</v>
@@ -6680,7 +6680,7 @@
         <v>0.0525856444288743</v>
       </c>
       <c r="N129" t="n">
-        <v>0.0001210535342889649</v>
+        <v>1.210535342889649e-05</v>
       </c>
       <c r="O129" t="inlineStr"/>
       <c r="P129" t="n">
@@ -6701,7 +6701,7 @@
         <v>1</v>
       </c>
       <c r="E130" t="n">
-        <v>0.44152848</v>
+        <v>0.044152848</v>
       </c>
       <c r="F130" t="n">
         <v>10.5</v>
@@ -6728,7 +6728,7 @@
         <v>0.05273755777432246</v>
       </c>
       <c r="N130" t="n">
-        <v>0.0001661386366098395</v>
+        <v>1.661386366098395e-05</v>
       </c>
       <c r="O130" t="inlineStr"/>
       <c r="P130" t="n">
@@ -6749,16 +6749,16 @@
         <v>0.8</v>
       </c>
       <c r="E131" t="n">
-        <v>0.39601008</v>
+        <v>0.039601008</v>
       </c>
       <c r="F131" t="n">
         <v>8.4</v>
       </c>
       <c r="G131" t="n">
-        <v>1.098957082966697</v>
+        <v>0.1098957082966697</v>
       </c>
       <c r="H131" t="n">
-        <v>0.130828224162702</v>
+        <v>0.0130828224162702</v>
       </c>
       <c r="I131" t="n">
         <v>26.1</v>
@@ -6776,7 +6776,7 @@
         <v>0.05265216044950102</v>
       </c>
       <c r="N131" t="n">
-        <v>0.0001516691940041299</v>
+        <v>1.516691940041299e-05</v>
       </c>
       <c r="O131" t="inlineStr"/>
       <c r="P131" t="n">
@@ -6797,16 +6797,16 @@
         <v>0.15</v>
       </c>
       <c r="E132" t="n">
-        <v>0.045945135</v>
+        <v>0.004594513499999999</v>
       </c>
       <c r="F132" t="n">
         <v>1.575</v>
       </c>
       <c r="G132" t="n">
-        <v>0.6033449560819195</v>
+        <v>0.06033449560819195</v>
       </c>
       <c r="H132" t="n">
-        <v>0.3830761625916949</v>
+        <v>0.03830761625916949</v>
       </c>
       <c r="I132" t="n">
         <v>26.1</v>
@@ -6824,7 +6824,7 @@
         <v>0.05250535686956141</v>
       </c>
       <c r="N132" t="n">
-        <v>4.547011198045832e-05</v>
+        <v>4.547011198045831e-06</v>
       </c>
       <c r="O132" t="inlineStr"/>
       <c r="P132" t="n">
@@ -6845,16 +6845,16 @@
         <v>0.31</v>
       </c>
       <c r="E133" t="n">
-        <v>0.13285683</v>
+        <v>0.013285683</v>
       </c>
       <c r="F133" t="n">
         <v>3.255</v>
       </c>
       <c r="G133" t="n">
-        <v>1.360665454009564</v>
+        <v>0.1360665454009563</v>
       </c>
       <c r="H133" t="n">
-        <v>0.4180231809553192</v>
+        <v>0.0418023180955319</v>
       </c>
       <c r="I133" t="n">
         <v>26.1</v>
@@ -6872,7 +6872,7 @@
         <v>0.05252287596847682</v>
       </c>
       <c r="N133" t="n">
-        <v>7.372560337072021e-05</v>
+        <v>7.372560337072019e-06</v>
       </c>
       <c r="O133" t="inlineStr"/>
       <c r="P133" t="n">
@@ -6893,16 +6893,16 @@
         <v>0.61</v>
       </c>
       <c r="E134" t="n">
-        <v>0.31066308</v>
+        <v>0.031066308</v>
       </c>
       <c r="F134" t="n">
         <v>6.405</v>
       </c>
       <c r="G134" t="n">
-        <v>1.753505073599009</v>
+        <v>0.1753505073599008</v>
       </c>
       <c r="H134" t="n">
-        <v>0.2737712839342715</v>
+        <v>0.02737712839342714</v>
       </c>
       <c r="I134" t="n">
         <v>26.1</v>
@@ -6920,7 +6920,7 @@
         <v>0.05258852061049066</v>
       </c>
       <c r="N134" t="n">
-        <v>0.0001251586105756037</v>
+        <v>1.251586105756037e-05</v>
       </c>
       <c r="O134" t="inlineStr"/>
       <c r="P134" t="n">
@@ -6941,16 +6941,16 @@
         <v>0.85</v>
       </c>
       <c r="E135" t="n">
-        <v>0.01479348</v>
+        <v>0.001479348</v>
       </c>
       <c r="F135" t="n">
         <v>8.924999999999999</v>
       </c>
       <c r="G135" t="n">
-        <v>0.03872924007418961</v>
+        <v>0.003872924007418961</v>
       </c>
       <c r="H135" t="n">
-        <v>0.004339410652570265</v>
+        <v>0.0004339410652570265</v>
       </c>
       <c r="I135" t="n">
         <v>26.1</v>
@@ -6968,7 +6968,7 @@
         <v>0.05267174289882574</v>
       </c>
       <c r="N135" t="n">
-        <v>2.367101177284478e-05</v>
+        <v>2.367101177284478e-06</v>
       </c>
       <c r="O135" t="inlineStr"/>
       <c r="P135" t="n">
@@ -6989,16 +6989,16 @@
         <v>0.12</v>
       </c>
       <c r="E136" t="n">
-        <v>-0.0100292535</v>
+        <v>-0.00100292535</v>
       </c>
       <c r="F136" t="n">
         <v>1.32</v>
       </c>
       <c r="G136" t="n">
-        <v>-0.1412601005393773</v>
+        <v>-0.01412601005393772</v>
       </c>
       <c r="H136" t="n">
-        <v>-0.1070152276813464</v>
+        <v>-0.01070152276813464</v>
       </c>
       <c r="I136" t="n">
         <v>25.8</v>
@@ -7016,7 +7016,7 @@
         <v>0.05500327262990812</v>
       </c>
       <c r="N136" t="n">
-        <v>-1.461478750632609e-05</v>
+        <v>-1.461478750632609e-06</v>
       </c>
       <c r="O136" t="inlineStr">
         <is>
@@ -7041,16 +7041,16 @@
         <v>0.73</v>
       </c>
       <c r="E137" t="n">
-        <v>0.33053554035</v>
+        <v>0.033053554035</v>
       </c>
       <c r="F137" t="n">
         <v>8.029999999999999</v>
       </c>
       <c r="G137" t="n">
-        <v>1.533382517380181</v>
+        <v>0.1533382517380181</v>
       </c>
       <c r="H137" t="n">
-        <v>0.1909567269464734</v>
+        <v>0.01909567269464734</v>
       </c>
       <c r="I137" t="n">
         <v>25.8</v>
@@ -7068,7 +7068,7 @@
         <v>0.05512098057908622</v>
       </c>
       <c r="N137" t="n">
-        <v>0.000128334011886687</v>
+        <v>1.28334011886687e-05</v>
       </c>
       <c r="O137" t="inlineStr"/>
       <c r="P137" t="n">
@@ -7089,16 +7089,16 @@
         <v>0.145</v>
       </c>
       <c r="E138" t="n">
-        <v>0.003438601200000009</v>
+        <v>0.0003438601200000008</v>
       </c>
       <c r="F138" t="n">
         <v>1.595</v>
       </c>
       <c r="G138" t="n">
-        <v>0.04695566762060926</v>
+        <v>0.004695566762060925</v>
       </c>
       <c r="H138" t="n">
-        <v>0.02943929004426913</v>
+        <v>0.002943929004426912</v>
       </c>
       <c r="I138" t="n">
         <v>25.8</v>
@@ -7116,7 +7116,7 @@
         <v>0.05500477820153447</v>
       </c>
       <c r="N138" t="n">
-        <v>4.022424762799586e-06</v>
+        <v>4.022424762799585e-07</v>
       </c>
       <c r="O138" t="inlineStr"/>
       <c r="P138" t="n">
@@ -7137,16 +7137,16 @@
         <v>0.18</v>
       </c>
       <c r="E139" t="n">
-        <v>0.013539492225</v>
+        <v>0.0013539492225</v>
       </c>
       <c r="F139" t="n">
         <v>1.98</v>
       </c>
       <c r="G139" t="n">
-        <v>0.1758136864705707</v>
+        <v>0.01758136864705707</v>
       </c>
       <c r="H139" t="n">
-        <v>0.08879479114675289</v>
+        <v>0.008879479114675288</v>
       </c>
       <c r="I139" t="n">
         <v>25.8</v>
@@ -7164,7 +7164,7 @@
         <v>0.05500736314349198</v>
       </c>
       <c r="N139" t="n">
-        <v>1.387856206794674e-05</v>
+        <v>1.387856206794674e-06</v>
       </c>
       <c r="O139" t="inlineStr"/>
       <c r="P139" t="n">
@@ -7185,16 +7185,16 @@
         <v>0.21</v>
       </c>
       <c r="E140" t="n">
-        <v>0.02851173495000001</v>
+        <v>0.002851173495</v>
       </c>
       <c r="F140" t="n">
         <v>2.31</v>
       </c>
       <c r="G140" t="n">
-        <v>0.3582890282400776</v>
+        <v>0.03582890282400775</v>
       </c>
       <c r="H140" t="n">
-        <v>0.155103475428605</v>
+        <v>0.0155103475428605</v>
       </c>
       <c r="I140" t="n">
         <v>25.8</v>
@@ -7212,7 +7212,7 @@
         <v>0.05501002181421128</v>
       </c>
       <c r="N140" t="n">
-        <v>2.491134462463197e-05</v>
+        <v>2.491134462463196e-06</v>
       </c>
       <c r="O140" t="inlineStr"/>
       <c r="P140" t="n">
@@ -7233,16 +7233,16 @@
         <v>0.27</v>
       </c>
       <c r="E141" t="n">
-        <v>0.06289774695000001</v>
+        <v>0.006289774695</v>
       </c>
       <c r="F141" t="n">
         <v>2.97</v>
       </c>
       <c r="G141" t="n">
-        <v>0.7278233507291474</v>
+        <v>0.07278233507291472</v>
       </c>
       <c r="H141" t="n">
-        <v>0.2450583672488711</v>
+        <v>0.02450583672488711</v>
       </c>
       <c r="I141" t="n">
         <v>25.8</v>
@@ -7260,7 +7260,7 @@
         <v>0.05501656568707283</v>
       </c>
       <c r="N141" t="n">
-        <v>4.236415789825499e-05</v>
+        <v>4.236415789825498e-06</v>
       </c>
       <c r="O141" t="inlineStr"/>
       <c r="P141" t="n">
@@ -7281,16 +7281,16 @@
         <v>0.34</v>
       </c>
       <c r="E142" t="n">
-        <v>0.10272821085</v>
+        <v>0.010272821085</v>
       </c>
       <c r="F142" t="n">
         <v>3.74</v>
       </c>
       <c r="G142" t="n">
-        <v>1.066085402633594</v>
+        <v>0.1066085402633594</v>
       </c>
       <c r="H142" t="n">
-        <v>0.2850495728966829</v>
+        <v>0.02850495728966829</v>
       </c>
       <c r="I142" t="n">
         <v>25.8</v>
@@ -7308,7 +7308,7 @@
         <v>0.0550262664552121</v>
       </c>
       <c r="N142" t="n">
-        <v>5.715690795572146e-05</v>
+        <v>5.715690795572146e-06</v>
       </c>
       <c r="O142" t="inlineStr"/>
       <c r="P142" t="n">
@@ -7329,16 +7329,16 @@
         <v>0.39</v>
       </c>
       <c r="E143" t="n">
-        <v>0.12995047035</v>
+        <v>0.012995047035</v>
       </c>
       <c r="F143" t="n">
         <v>4.29</v>
       </c>
       <c r="G143" t="n">
-        <v>1.242445224808853</v>
+        <v>0.1242445224808852</v>
       </c>
       <c r="H143" t="n">
-        <v>0.2896142715172151</v>
+        <v>0.0289614271517215</v>
       </c>
       <c r="I143" t="n">
         <v>25.8</v>
@@ -7356,7 +7356,7 @@
         <v>0.05503455732537511</v>
       </c>
       <c r="N143" t="n">
-        <v>6.607483362026046e-05</v>
+        <v>6.607483362026044e-06</v>
       </c>
       <c r="O143" t="inlineStr"/>
       <c r="P143" t="n">
@@ -7377,16 +7377,16 @@
         <v>0.46</v>
       </c>
       <c r="E144" t="n">
-        <v>0.1621873566000001</v>
+        <v>0.01621873566</v>
       </c>
       <c r="F144" t="n">
         <v>5.06</v>
       </c>
       <c r="G144" t="n">
-        <v>1.41988081429252</v>
+        <v>0.141988081429252</v>
       </c>
       <c r="H144" t="n">
-        <v>0.2806088565795494</v>
+        <v>0.02806088565795493</v>
       </c>
       <c r="I144" t="n">
         <v>25.8</v>
@@ -7404,7 +7404,7 @@
         <v>0.05504806990258605</v>
       </c>
       <c r="N144" t="n">
-        <v>7.617501186748045e-05</v>
+        <v>7.617501186748042e-06</v>
       </c>
       <c r="O144" t="inlineStr"/>
       <c r="P144" t="n">
@@ -7425,16 +7425,16 @@
         <v>0.49</v>
       </c>
       <c r="E145" t="n">
-        <v>0.1836786141</v>
+        <v>0.01836786141</v>
       </c>
       <c r="F145" t="n">
         <v>5.39</v>
       </c>
       <c r="G145" t="n">
-        <v>1.513777145805588</v>
+        <v>0.1513777145805587</v>
       </c>
       <c r="H145" t="n">
-        <v>0.2808491921717231</v>
+        <v>0.02808491921717231</v>
       </c>
       <c r="I145" t="n">
         <v>25.8</v>
@@ -7452,7 +7452,7 @@
         <v>0.0550545411387653</v>
       </c>
       <c r="N145" t="n">
-        <v>8.279833331028253e-05</v>
+        <v>8.279833331028252e-06</v>
       </c>
       <c r="O145" t="inlineStr"/>
       <c r="P145" t="n">
@@ -7473,16 +7473,16 @@
         <v>0.52</v>
       </c>
       <c r="E146" t="n">
-        <v>0.1922751171</v>
+        <v>0.01922751171</v>
       </c>
       <c r="F146" t="n">
         <v>5.720000000000001</v>
       </c>
       <c r="G146" t="n">
-        <v>1.540327743141167</v>
+        <v>0.1540327743141167</v>
       </c>
       <c r="H146" t="n">
-        <v>0.2692880669827215</v>
+        <v>0.02692880669827214</v>
       </c>
       <c r="I146" t="n">
         <v>25.8</v>
@@ -7500,7 +7500,7 @@
         <v>0.0550614202504803</v>
       </c>
       <c r="N146" t="n">
-        <v>8.543887741684228e-05</v>
+        <v>8.543887741684226e-06</v>
       </c>
       <c r="O146" t="inlineStr"/>
       <c r="P146" t="n">
@@ -7521,16 +7521,16 @@
         <v>0.54</v>
       </c>
       <c r="E147" t="n">
-        <v>0.21591550035</v>
+        <v>0.021591550035</v>
       </c>
       <c r="F147" t="n">
         <v>5.94</v>
       </c>
       <c r="G147" t="n">
-        <v>1.594048591784953</v>
+        <v>0.1594048591784952</v>
       </c>
       <c r="H147" t="n">
-        <v>0.2683583487853455</v>
+        <v>0.02683583487853455</v>
       </c>
       <c r="I147" t="n">
         <v>25.8</v>
@@ -7548,7 +7548,7 @@
         <v>0.05506623284736301</v>
       </c>
       <c r="N147" t="n">
-        <v>9.269753064970686e-05</v>
+        <v>9.269753064970685e-06</v>
       </c>
       <c r="O147" t="inlineStr"/>
       <c r="P147" t="n">
@@ -7569,16 +7569,16 @@
         <v>0.57</v>
       </c>
       <c r="E148" t="n">
-        <v>0.2223628776</v>
+        <v>0.02223628776</v>
       </c>
       <c r="F148" t="n">
         <v>6.27</v>
       </c>
       <c r="G148" t="n">
-        <v>1.588090611336287</v>
+        <v>0.1588090611336287</v>
       </c>
       <c r="H148" t="n">
-        <v>0.2532839890488496</v>
+        <v>0.02532839890488496</v>
       </c>
       <c r="I148" t="n">
         <v>25.8</v>
@@ -7596,7 +7596,7 @@
         <v>0.05507379140752887</v>
       </c>
       <c r="N148" t="n">
-        <v>9.467928167403688e-05</v>
+        <v>9.467928167403688e-06</v>
       </c>
       <c r="O148" t="inlineStr"/>
       <c r="P148" t="n">
@@ -7617,16 +7617,16 @@
         <v>0.6</v>
       </c>
       <c r="E149" t="n">
-        <v>0.27752377185</v>
+        <v>0.027752377185</v>
       </c>
       <c r="F149" t="n">
         <v>6.6</v>
       </c>
       <c r="G149" t="n">
-        <v>1.819295061393822</v>
+        <v>0.1819295061393822</v>
       </c>
       <c r="H149" t="n">
-        <v>0.2756507668778518</v>
+        <v>0.02756507668778518</v>
       </c>
       <c r="I149" t="n">
         <v>25.8</v>
@@ -7644,7 +7644,7 @@
         <v>0.05508175741568164</v>
       </c>
       <c r="N149" t="n">
-        <v>0.0001117318528275092</v>
+        <v>1.117318528275092e-05</v>
       </c>
       <c r="O149" t="inlineStr"/>
       <c r="P149" t="n">
@@ -7665,16 +7665,16 @@
         <v>0.62</v>
       </c>
       <c r="E150" t="n">
-        <v>0.24170500935</v>
+        <v>0.024170500935</v>
       </c>
       <c r="F150" t="n">
         <v>6.82</v>
       </c>
       <c r="G150" t="n">
-        <v>1.478179300395101</v>
+        <v>0.1478179300395101</v>
       </c>
       <c r="H150" t="n">
-        <v>0.2167418329025075</v>
+        <v>0.02167418329025074</v>
       </c>
       <c r="I150" t="n">
         <v>25.8</v>
@@ -7692,7 +7692,7 @@
         <v>0.05508729436085966</v>
       </c>
       <c r="N150" t="n">
-        <v>0.0001006363351997667</v>
+        <v>1.006363351997667e-05</v>
       </c>
       <c r="O150" t="inlineStr"/>
       <c r="P150" t="n">
@@ -7713,16 +7713,16 @@
         <v>0.66</v>
       </c>
       <c r="E151" t="n">
-        <v>0.25889801535</v>
+        <v>0.025889801535</v>
       </c>
       <c r="F151" t="n">
         <v>7.260000000000001</v>
       </c>
       <c r="G151" t="n">
-        <v>1.426077354018783</v>
+        <v>0.1426077354018782</v>
       </c>
       <c r="H151" t="n">
-        <v>0.1964293876058929</v>
+        <v>0.01964293876058929</v>
       </c>
       <c r="I151" t="n">
         <v>25.8</v>
@@ -7740,7 +7740,7 @@
         <v>0.05509891106002006</v>
       </c>
       <c r="N151" t="n">
-        <v>0.0001059506652933467</v>
+        <v>1.059506652933466e-05</v>
       </c>
       <c r="O151" t="inlineStr"/>
       <c r="P151" t="n">
@@ -7761,16 +7761,16 @@
         <v>0.6899999999999999</v>
       </c>
       <c r="E152" t="n">
-        <v>0.28038927285</v>
+        <v>0.028038927285</v>
       </c>
       <c r="F152" t="n">
         <v>7.59</v>
       </c>
       <c r="G152" t="n">
-        <v>1.388836600375789</v>
+        <v>0.1388836600375788</v>
       </c>
       <c r="H152" t="n">
-        <v>0.1829824242919353</v>
+        <v>0.01829824242919352</v>
       </c>
       <c r="I152" t="n">
         <v>25.8</v>
@@ -7788,7 +7788,7 @@
         <v>0.05510809831594628</v>
       </c>
       <c r="N152" t="n">
-        <v>0.0001126236154714265</v>
+        <v>1.126236154714265e-05</v>
       </c>
       <c r="O152" t="inlineStr"/>
       <c r="P152" t="n">
@@ -7809,16 +7809,16 @@
         <v>0.72</v>
       </c>
       <c r="E153" t="n">
-        <v>0.29328402735</v>
+        <v>0.029328402735</v>
       </c>
       <c r="F153" t="n">
         <v>7.92</v>
       </c>
       <c r="G153" t="n">
-        <v>1.243861576746284</v>
+        <v>0.1243861576746284</v>
       </c>
       <c r="H153" t="n">
-        <v>0.157053229387157</v>
+        <v>0.0157053229387157</v>
       </c>
       <c r="I153" t="n">
         <v>25.8</v>
@@ -7836,7 +7836,7 @@
         <v>0.05511769225938256</v>
       </c>
       <c r="N153" t="n">
-        <v>0.0001166445049204666</v>
+        <v>1.166445049204665e-05</v>
       </c>
       <c r="O153" t="inlineStr"/>
       <c r="P153" t="n">
@@ -7857,16 +7857,16 @@
         <v>0.79</v>
       </c>
       <c r="E154" t="n">
-        <v>0.3140589096</v>
+        <v>0.03140589096</v>
       </c>
       <c r="F154" t="n">
         <v>8.690000000000001</v>
       </c>
       <c r="G154" t="n">
-        <v>1.14121957209414</v>
+        <v>0.114121957209414</v>
       </c>
       <c r="H154" t="n">
-        <v>0.1313256124389114</v>
+        <v>0.01313256124389114</v>
       </c>
       <c r="I154" t="n">
         <v>25.8</v>
@@ -7884,7 +7884,7 @@
         <v>0.05514165848068047</v>
       </c>
       <c r="N154" t="n">
-        <v>0.0001231502225938371</v>
+        <v>1.231502225938371e-05</v>
       </c>
       <c r="O154" t="inlineStr"/>
       <c r="P154" t="n">
@@ -7905,16 +7905,16 @@
         <v>0.67</v>
       </c>
       <c r="E155" t="n">
-        <v>0.27036001935</v>
+        <v>0.02703600193499999</v>
       </c>
       <c r="F155" t="n">
         <v>7.37</v>
       </c>
       <c r="G155" t="n">
-        <v>1.319340831954297</v>
+        <v>0.1319340831954297</v>
       </c>
       <c r="H155" t="n">
-        <v>0.1790150382570281</v>
+        <v>0.01790150382570281</v>
       </c>
       <c r="I155" t="n">
         <v>25.8</v>
@@ -7932,7 +7932,7 @@
         <v>0.05510192827841871</v>
       </c>
       <c r="N155" t="n">
-        <v>0.0001095052196449467</v>
+        <v>1.095052196449467e-05</v>
       </c>
       <c r="O155" t="inlineStr"/>
       <c r="P155" t="n">

</xml_diff>